<commit_message>
add some fun rare HDMI formats
</commit_message>
<xml_diff>
--- a/display-pixel-ratios.xlsx
+++ b/display-pixel-ratios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="98">
   <si>
     <t xml:space="preserve">CINEMA DCP 4k</t>
   </si>
@@ -241,13 +241,16 @@
     <t xml:space="preserve">1080p</t>
   </si>
   <si>
+    <t xml:space="preserve">HDMI “21:9” aka 7:3 aka 64:27</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.66:1 (5:3)  /  1920x1152</t>
   </si>
   <si>
     <t xml:space="preserve">1.77:1 (16:9)  /  1920x1080</t>
   </si>
   <si>
-    <t xml:space="preserve">ATSC-1080p</t>
+    <t xml:space="preserve">HDMI-1080p</t>
   </si>
   <si>
     <t xml:space="preserve">1.85:1  /  1920x1038</t>
@@ -292,7 +295,7 @@
     <t xml:space="preserve">1.77:1 (16:9)  /  1280x720</t>
   </si>
   <si>
-    <t xml:space="preserve">ATSC-720p</t>
+    <t xml:space="preserve">HDMI-720p</t>
   </si>
   <si>
     <t xml:space="preserve">1.85:1  /  1280x692</t>
@@ -326,6 +329,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -347,6 +351,7 @@
       <sz val="16"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -354,11 +359,13 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -403,13 +410,9 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -428,11 +431,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -457,68 +460,68 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L109"/>
+  <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I64" activeCellId="0" sqref="I64"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K85" activeCellId="0" sqref="K85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.92"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="8.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="4.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="4.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="8.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="6.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="4.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="4.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="6.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4"/>
+      <c r="A1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="53.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="5"/>
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="6" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="6"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="1" t="n">
         <f aca="false">E4/F4</f>
         <v>1.85</v>
       </c>
@@ -531,29 +534,29 @@
       <c r="F4" s="1" t="n">
         <v>2160</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="2" t="n">
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1" t="n">
         <f aca="false">LCM(E4*H4,F4*G4)/(F4*G4)</f>
         <v>37</v>
       </c>
-      <c r="J4" s="2" t="n">
+      <c r="J4" s="1" t="n">
         <f aca="false">LCM(E4*H4,F4*G4)/(E4*H4)</f>
         <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="1" t="n">
         <f aca="false">E5/F5</f>
         <v>2.38694638694639</v>
       </c>
@@ -566,27 +569,27 @@
       <c r="F5" s="1" t="n">
         <v>1716</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="2" t="n">
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="1" t="n">
         <f aca="false">LCM(E5*H5,F5*G5)/(F5*G5)</f>
         <v>1024</v>
       </c>
-      <c r="J5" s="2" t="n">
+      <c r="J5" s="1" t="n">
         <f aca="false">LCM(E5*H5,F5*G5)/(E5*H5)</f>
         <v>429</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="1" t="n">
         <f aca="false">E6/F6</f>
         <v>2.38694638694639</v>
       </c>
@@ -601,27 +604,27 @@
         <f aca="false">F5</f>
         <v>1716</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="2" t="n">
+      <c r="I6" s="1" t="n">
         <f aca="false">LCM(E6*H6,F6*G6)/(F6*G6)</f>
         <v>192</v>
       </c>
-      <c r="J6" s="2" t="n">
+      <c r="J6" s="1" t="n">
         <f aca="false">LCM(E6*H6,F6*G6)/(E6*H6)</f>
         <v>143</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="1" t="n">
         <f aca="false">E7/F7</f>
         <v>2.38694638694639</v>
       </c>
@@ -636,29 +639,29 @@
         <f aca="false">F5</f>
         <v>1716</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="2" t="n">
+      <c r="I7" s="1" t="n">
         <f aca="false">LCM(E7*H7,F7*G7)/(F7*G7)</f>
         <v>256</v>
       </c>
-      <c r="J7" s="2" t="n">
+      <c r="J7" s="1" t="n">
         <f aca="false">LCM(E7*H7,F7*G7)/(E7*H7)</f>
         <v>143</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="1" t="n">
         <f aca="false">LCM(E8,F8)/F8</f>
         <v>16</v>
       </c>
@@ -678,23 +681,23 @@
       <c r="H8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="2" t="n">
+      <c r="I8" s="1" t="n">
         <f aca="false">LCM(E8*H8,F8*G8)/(F8*G8)</f>
         <v>16</v>
       </c>
-      <c r="J8" s="2" t="n">
+      <c r="J8" s="1" t="n">
         <f aca="false">LCM(E8*H8,F8*G8)/(E8*H8)</f>
         <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" s="1" t="n">
         <f aca="false">E9/F9</f>
         <v>1.8962962962963</v>
       </c>
@@ -707,27 +710,27 @@
       <c r="F9" s="1" t="n">
         <v>2160</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="2" t="n">
+      <c r="G9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="1" t="n">
         <f aca="false">LCM(E9*H9,F9*G9)/(F9*G9)</f>
         <v>256</v>
       </c>
-      <c r="J9" s="2" t="n">
+      <c r="J9" s="1" t="n">
         <f aca="false">LCM(E9*H9,F9*G9)/(E9*H9)</f>
         <v>135</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="1" t="n">
         <f aca="false">E10/F10</f>
         <v>1.8962962962963</v>
       </c>
@@ -742,27 +745,27 @@
         <f aca="false">F9</f>
         <v>2160</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="2" t="n">
+      <c r="I10" s="1" t="n">
         <f aca="false">LCM(E10*H10,F10*G10)/(F10*G10)</f>
         <v>16</v>
       </c>
-      <c r="J10" s="2" t="n">
+      <c r="J10" s="1" t="n">
         <f aca="false">LCM(E10*H10,F10*G10)/(E10*H10)</f>
         <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" s="1" t="n">
         <v>1.8962962962963</v>
       </c>
       <c r="D11" s="1" t="n">
@@ -776,39 +779,39 @@
         <f aca="false">F9</f>
         <v>2160</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="2" t="n">
+      <c r="I11" s="1" t="n">
         <f aca="false">LCM(E11*H11,F11*G11)/(F11*G11)</f>
         <v>64</v>
       </c>
-      <c r="J11" s="2" t="n">
+      <c r="J11" s="1" t="n">
         <f aca="false">LCM(E11*H11,F11*G11)/(E11*H11)</f>
         <v>45</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="C14" s="1" t="n">
         <f aca="false">E14/F14</f>
         <v>1.85</v>
       </c>
@@ -821,29 +824,29 @@
       <c r="F14" s="1" t="n">
         <v>1080</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="2" t="n">
+      <c r="G14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="1" t="n">
         <f aca="false">LCM(E14*H14,F14*G14)/(F14*G14)</f>
         <v>37</v>
       </c>
-      <c r="J14" s="2" t="n">
+      <c r="J14" s="1" t="n">
         <f aca="false">LCM(E14*H14,F14*G14)/(E14*H14)</f>
         <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="C15" s="1" t="n">
         <f aca="false">E15/F15</f>
         <v>2.38694638694639</v>
       </c>
@@ -856,27 +859,27 @@
       <c r="F15" s="1" t="n">
         <v>858</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="2" t="n">
+      <c r="G15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="1" t="n">
         <f aca="false">LCM(E15*H15,F15*G15)/(F15*G15)</f>
         <v>1024</v>
       </c>
-      <c r="J15" s="2" t="n">
+      <c r="J15" s="1" t="n">
         <f aca="false">LCM(E15*H15,F15*G15)/(E15*H15)</f>
         <v>429</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="2" t="n">
+      <c r="C16" s="1" t="n">
         <f aca="false">E16/F16</f>
         <v>2.38694638694639</v>
       </c>
@@ -889,27 +892,27 @@
       <c r="F16" s="1" t="n">
         <v>858</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="2" t="n">
+      <c r="I16" s="1" t="n">
         <f aca="false">LCM(E16*H16,F16*G16)/(F16*G16)</f>
         <v>192</v>
       </c>
-      <c r="J16" s="2" t="n">
+      <c r="J16" s="1" t="n">
         <f aca="false">LCM(E16*H16,F16*G16)/(E16*H16)</f>
         <v>143</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="2" t="n">
+      <c r="C17" s="1" t="n">
         <f aca="false">E17/F17</f>
         <v>2.38694638694639</v>
       </c>
@@ -922,29 +925,29 @@
       <c r="F17" s="1" t="n">
         <v>858</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="2" t="n">
+      <c r="I17" s="1" t="n">
         <f aca="false">LCM(E17*H17,F17*G17)/(F17*G17)</f>
         <v>256</v>
       </c>
-      <c r="J17" s="2" t="n">
+      <c r="J17" s="1" t="n">
         <f aca="false">LCM(E17*H17,F17*G17)/(E17*H17)</f>
         <v>143</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="2" t="n">
+      <c r="C18" s="1" t="n">
         <f aca="false">LCM(E18,F18)/F18</f>
         <v>16</v>
       </c>
@@ -958,29 +961,29 @@
       <c r="F18" s="1" t="n">
         <v>1080</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="2" t="n">
+      <c r="G18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="1" t="n">
         <f aca="false">LCM(E18*H18,F18*G18)/(F18*G18)</f>
         <v>16</v>
       </c>
-      <c r="J18" s="2" t="n">
+      <c r="J18" s="1" t="n">
         <f aca="false">LCM(E18*H18,F18*G18)/(E18*H18)</f>
         <v>9</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="2" t="n">
+      <c r="C19" s="1" t="n">
         <f aca="false">E19/F19</f>
         <v>1.8962962962963</v>
       </c>
@@ -993,27 +996,27 @@
       <c r="F19" s="1" t="n">
         <v>1080</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I19" s="2" t="n">
+      <c r="G19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="1" t="n">
         <f aca="false">LCM(E19*H19,F19*G19)/(F19*G19)</f>
         <v>256</v>
       </c>
-      <c r="J19" s="2" t="n">
+      <c r="J19" s="1" t="n">
         <f aca="false">LCM(E19*H19,F19*G19)/(E19*H19)</f>
         <v>135</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="2" t="n">
+      <c r="C20" s="1" t="n">
         <f aca="false">E20/F20</f>
         <v>1.8962962962963</v>
       </c>
@@ -1026,27 +1029,27 @@
       <c r="F20" s="1" t="n">
         <v>1080</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="2" t="n">
+      <c r="I20" s="1" t="n">
         <f aca="false">LCM(E20*H20,F20*G20)/(F20*G20)</f>
         <v>16</v>
       </c>
-      <c r="J20" s="2" t="n">
+      <c r="J20" s="1" t="n">
         <f aca="false">LCM(E20*H20,F20*G20)/(E20*H20)</f>
         <v>15</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8"/>
+      <c r="A21" s="7"/>
       <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="2" t="n">
+      <c r="C21" s="1" t="n">
         <f aca="false">E21/F21</f>
         <v>1.8962962962963</v>
       </c>
@@ -1059,36 +1062,36 @@
       <c r="F21" s="1" t="n">
         <v>1080</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I21" s="2" t="n">
+      <c r="I21" s="1" t="n">
         <f aca="false">LCM(E21*H21,F21*G21)/(F21*G21)</f>
         <v>64</v>
       </c>
-      <c r="J21" s="2" t="n">
+      <c r="J21" s="1" t="n">
         <f aca="false">LCM(E21*H21,F21*G21)/(E21*H21)</f>
         <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="2" t="n">
+      <c r="C24" s="1" t="n">
         <f aca="false">LCM(E24,F24)/F24</f>
         <v>4</v>
       </c>
@@ -1102,26 +1105,26 @@
       <c r="F24" s="1" t="n">
         <v>3840</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I24" s="2" t="n">
+      <c r="G24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="1" t="n">
         <f aca="false">LCM(E24*H24,F24*G24)/(F24*G24)</f>
         <v>4</v>
       </c>
-      <c r="J24" s="2" t="n">
+      <c r="J24" s="1" t="n">
         <f aca="false">LCM(E24*H24,F24*G24)/(E24*H24)</f>
         <v>3</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="2" t="n">
+      <c r="C25" s="1" t="n">
         <f aca="false">LCM(E25,F25)/F25</f>
         <v>5</v>
       </c>
@@ -1135,26 +1138,26 @@
       <c r="F25" s="1" t="n">
         <v>3072</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I25" s="2" t="n">
+      <c r="G25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="1" t="n">
         <f aca="false">LCM(E25*H25,F25*G25)/(F25*G25)</f>
         <v>5</v>
       </c>
-      <c r="J25" s="2" t="n">
+      <c r="J25" s="1" t="n">
         <f aca="false">LCM(E25*H25,F25*G25)/(E25*H25)</f>
         <v>3</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="2" t="n">
+      <c r="C26" s="1" t="n">
         <f aca="false">LCM(E26,F26)/F26</f>
         <v>16</v>
       </c>
@@ -1168,29 +1171,29 @@
       <c r="F26" s="1" t="n">
         <v>2880</v>
       </c>
-      <c r="G26" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I26" s="2" t="n">
+      <c r="G26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="1" t="n">
         <f aca="false">LCM(E26*H26,F26*G26)/(F26*G26)</f>
         <v>16</v>
       </c>
-      <c r="J26" s="2" t="n">
+      <c r="J26" s="1" t="n">
         <f aca="false">LCM(E26*H26,F26*G26)/(E26*H26)</f>
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="2" t="n">
+      <c r="C27" s="1" t="n">
         <f aca="false">E27/F27</f>
         <v>1.84971098265896</v>
       </c>
@@ -1203,29 +1206,29 @@
       <c r="F27" s="1" t="n">
         <v>2768</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I27" s="2" t="n">
+      <c r="G27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="1" t="n">
         <f aca="false">LCM(E27*H27,F27*G27)/(F27*G27)</f>
         <v>320</v>
       </c>
-      <c r="J27" s="2" t="n">
+      <c r="J27" s="1" t="n">
         <f aca="false">LCM(E27*H27,F27*G27)/(E27*H27)</f>
         <v>173</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="2" t="n">
+      <c r="C28" s="1" t="n">
         <f aca="false">E28/F28</f>
         <v>1.8962962962963</v>
       </c>
@@ -1238,27 +1241,27 @@
       <c r="F28" s="1" t="n">
         <v>2700</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I28" s="2" t="n">
+      <c r="G28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="1" t="n">
         <f aca="false">LCM(E28*H28,F28*G28)/(F28*G28)</f>
         <v>256</v>
       </c>
-      <c r="J28" s="2" t="n">
+      <c r="J28" s="1" t="n">
         <f aca="false">LCM(E28*H28,F28*G28)/(E28*H28)</f>
         <v>135</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="2" t="n">
+      <c r="C29" s="1" t="n">
         <f aca="false">E29/F29</f>
         <v>1.8962962962963</v>
       </c>
@@ -1271,27 +1274,27 @@
       <c r="F29" s="1" t="n">
         <v>2700</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I29" s="2" t="n">
+      <c r="I29" s="1" t="n">
         <f aca="false">LCM(E29*H29,F29*G29)/(F29*G29)</f>
         <v>16</v>
       </c>
-      <c r="J29" s="2" t="n">
+      <c r="J29" s="1" t="n">
         <f aca="false">LCM(E29*H29,F29*G29)/(E29*H29)</f>
         <v>15</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8"/>
+      <c r="A30" s="7"/>
       <c r="B30" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="2" t="n">
+      <c r="C30" s="1" t="n">
         <f aca="false">E30/F30</f>
         <v>1.8962962962963</v>
       </c>
@@ -1304,26 +1307,26 @@
       <c r="F30" s="1" t="n">
         <v>2700</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="2" t="n">
+      <c r="I30" s="1" t="n">
         <f aca="false">LCM(E30*H30,F30*G30)/(F30*G30)</f>
         <v>64</v>
       </c>
-      <c r="J30" s="2" t="n">
+      <c r="J30" s="1" t="n">
         <f aca="false">LCM(E30*H30,F30*G30)/(E30*H30)</f>
         <v>45</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="2" t="n">
+      <c r="C31" s="1" t="n">
         <f aca="false">LCM(E31,F31)/F31</f>
         <v>2</v>
       </c>
@@ -1337,29 +1340,29 @@
       <c r="F31" s="1" t="n">
         <v>2560</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I31" s="2" t="n">
+      <c r="G31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" s="1" t="n">
         <f aca="false">LCM(E31*H31,F31*G31)/(F31*G31)</f>
         <v>2</v>
       </c>
-      <c r="J31" s="2" t="n">
+      <c r="J31" s="1" t="n">
         <f aca="false">LCM(E31*H31,F31*G31)/(E31*H31)</f>
         <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="2" t="n">
+      <c r="C32" s="1" t="n">
         <f aca="false">E32/F32</f>
         <v>2.37037037037037</v>
       </c>
@@ -1372,27 +1375,27 @@
       <c r="F32" s="1" t="n">
         <v>2160</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I32" s="2" t="n">
+      <c r="G32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" s="1" t="n">
         <f aca="false">LCM(E32*H32,F32*G32)/(F32*G32)</f>
         <v>64</v>
       </c>
-      <c r="J32" s="2" t="n">
+      <c r="J32" s="1" t="n">
         <f aca="false">LCM(E32*H32,F32*G32)/(E32*H32)</f>
         <v>27</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="2" t="n">
+      <c r="C33" s="1" t="n">
         <f aca="false">E33/F33</f>
         <v>2.37037037037037</v>
       </c>
@@ -1405,27 +1408,27 @@
       <c r="F33" s="1" t="n">
         <v>2160</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="G33" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I33" s="2" t="n">
+      <c r="I33" s="1" t="n">
         <f aca="false">LCM(E33*H33,F33*G33)/(F33*G33)</f>
         <v>4</v>
       </c>
-      <c r="J33" s="2" t="n">
+      <c r="J33" s="1" t="n">
         <f aca="false">LCM(E33*H33,F33*G33)/(E33*H33)</f>
         <v>3</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8"/>
+      <c r="A34" s="7"/>
       <c r="B34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="2" t="n">
+      <c r="C34" s="1" t="n">
         <f aca="false">E34/F34</f>
         <v>2.37037037037037</v>
       </c>
@@ -1438,26 +1441,26 @@
       <c r="F34" s="1" t="n">
         <v>2160</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I34" s="2" t="n">
+      <c r="I34" s="1" t="n">
         <f aca="false">LCM(E34*H34,F34*G34)/(F34*G34)</f>
         <v>16</v>
       </c>
-      <c r="J34" s="2" t="n">
+      <c r="J34" s="1" t="n">
         <f aca="false">LCM(E34*H34,F34*G34)/(E34*H34)</f>
         <v>9</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="2" t="n">
+      <c r="C35" s="1" t="n">
         <f aca="false">E35/F35</f>
         <v>2.39028944911298</v>
       </c>
@@ -1470,17 +1473,17 @@
       <c r="F35" s="1" t="n">
         <v>2142</v>
       </c>
-      <c r="G35" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I35" s="2" t="n">
+      <c r="G35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" s="1" t="n">
         <f aca="false">LCM(E35*H35,F35*G35)/(F35*G35)</f>
         <v>2560</v>
       </c>
-      <c r="J35" s="2" t="n">
+      <c r="J35" s="1" t="n">
         <f aca="false">LCM(E35*H35,F35*G35)/(E35*H35)</f>
         <v>1071</v>
       </c>
@@ -1490,8 +1493,8 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8"/>
-      <c r="C36" s="2" t="n">
+      <c r="A36" s="7"/>
+      <c r="C36" s="1" t="n">
         <f aca="false">E36/F36</f>
         <v>2.39028944911298</v>
       </c>
@@ -1504,24 +1507,24 @@
       <c r="F36" s="1" t="n">
         <v>2142</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="G36" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="H36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I36" s="2" t="n">
+      <c r="I36" s="1" t="n">
         <f aca="false">LCM(E36*H36,F36*G36)/(F36*G36)</f>
         <v>160</v>
       </c>
-      <c r="J36" s="2" t="n">
+      <c r="J36" s="1" t="n">
         <f aca="false">LCM(E36*H36,F36*G36)/(E36*H36)</f>
         <v>119</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="8"/>
-      <c r="C37" s="2" t="n">
+      <c r="A37" s="7"/>
+      <c r="C37" s="1" t="n">
         <f aca="false">E37/F37</f>
         <v>2.39028944911298</v>
       </c>
@@ -1534,26 +1537,26 @@
       <c r="F37" s="1" t="n">
         <v>2142</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="H37" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I37" s="2" t="n">
+      <c r="I37" s="1" t="n">
         <f aca="false">LCM(E37*H37,F37*G37)/(F37*G37)</f>
         <v>640</v>
       </c>
-      <c r="J37" s="2" t="n">
+      <c r="J37" s="1" t="n">
         <f aca="false">LCM(E37*H37,F37*G37)/(E37*H37)</f>
         <v>357</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="2" t="n">
+      <c r="C38" s="1" t="n">
         <f aca="false">E38/F38</f>
         <v>2.40037505860291</v>
       </c>
@@ -1566,24 +1569,24 @@
       <c r="F38" s="1" t="n">
         <v>2133</v>
       </c>
-      <c r="G38" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I38" s="2" t="n">
+      <c r="G38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="1" t="n">
         <f aca="false">LCM(E38*H38,F38*G38)/(F38*G38)</f>
         <v>5120</v>
       </c>
-      <c r="J38" s="2" t="n">
+      <c r="J38" s="1" t="n">
         <f aca="false">LCM(E38*H38,F38*G38)/(E38*H38)</f>
         <v>2133</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="8"/>
-      <c r="C39" s="2" t="n">
+      <c r="A39" s="7"/>
+      <c r="C39" s="1" t="n">
         <f aca="false">E39/F39</f>
         <v>2.40037505860291</v>
       </c>
@@ -1596,26 +1599,26 @@
       <c r="F39" s="1" t="n">
         <v>2133</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="G39" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="H39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I39" s="2" t="n">
+      <c r="I39" s="1" t="n">
         <f aca="false">LCM(E39*H39,F39*G39)/(F39*G39)</f>
         <v>320</v>
       </c>
-      <c r="J39" s="2" t="n">
+      <c r="J39" s="1" t="n">
         <f aca="false">LCM(E39*H39,F39*G39)/(E39*H39)</f>
         <v>237</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="2" t="n">
+      <c r="C40" s="1" t="n">
         <f aca="false">E40/F40</f>
         <v>2.44041944709247</v>
       </c>
@@ -1628,27 +1631,27 @@
       <c r="F40" s="1" t="n">
         <v>2098</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I40" s="2" t="n">
+      <c r="G40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I40" s="1" t="n">
         <f aca="false">LCM(E40*H40,F40*G40)/(F40*G40)</f>
         <v>2560</v>
       </c>
-      <c r="J40" s="2" t="n">
+      <c r="J40" s="1" t="n">
         <f aca="false">LCM(E40*H40,F40*G40)/(E40*H40)</f>
         <v>1049</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B41" s="0"/>
-      <c r="C41" s="2" t="n">
+      <c r="C41" s="1" t="n">
         <f aca="false">E41/F41</f>
         <v>2.34970169802662</v>
       </c>
@@ -1661,27 +1664,27 @@
       <c r="F41" s="1" t="n">
         <v>2179</v>
       </c>
-      <c r="G41" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I41" s="2" t="n">
+      <c r="G41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I41" s="1" t="n">
         <f aca="false">LCM(E41*H41,F41*G41)/(F41*G41)</f>
         <v>5120</v>
       </c>
-      <c r="J41" s="2" t="n">
+      <c r="J41" s="1" t="n">
         <f aca="false">LCM(E41*H41,F41*G41)/(E41*H41)</f>
         <v>2179</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B42" s="0"/>
-      <c r="C42" s="2" t="n">
+      <c r="C42" s="1" t="n">
         <f aca="false">E42/F42</f>
         <v>2.34862385321101</v>
       </c>
@@ -1694,75 +1697,75 @@
       <c r="F42" s="1" t="n">
         <v>2180</v>
       </c>
-      <c r="G42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I42" s="2" t="n">
+      <c r="G42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I42" s="1" t="n">
         <f aca="false">LCM(E42*H42,F42*G42)/(F42*G42)</f>
         <v>256</v>
       </c>
-      <c r="J42" s="2" t="n">
+      <c r="J42" s="1" t="n">
         <f aca="false">LCM(E42*H42,F42*G42)/(E42*H42)</f>
         <v>109</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="7" t="s">
         <v>41</v>
       </c>
       <c r="E45" s="1" t="n">
         <v>4096</v>
       </c>
-      <c r="G45" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H45" s="3" t="s">
+      <c r="G45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="7" t="s">
         <v>42</v>
       </c>
       <c r="E46" s="1" t="n">
         <v>4096</v>
       </c>
-      <c r="G46" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H46" s="3" t="s">
+      <c r="G46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H46" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="7" t="s">
         <v>43</v>
       </c>
       <c r="E47" s="1" t="n">
         <v>4096</v>
       </c>
-      <c r="G47" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H47" s="3" t="s">
+      <c r="G47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H47" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="8" t="s">
+      <c r="A48" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -1771,151 +1774,151 @@
       <c r="E48" s="1" t="n">
         <v>4096</v>
       </c>
-      <c r="G48" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H48" s="3" t="s">
+      <c r="G48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E49" s="1" t="n">
         <v>4096</v>
       </c>
-      <c r="G49" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H49" s="3" t="s">
+      <c r="G49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="7" t="s">
         <v>46</v>
       </c>
       <c r="E50" s="1" t="n">
         <v>4096</v>
       </c>
-      <c r="G50" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H50" s="3" t="s">
+      <c r="G50" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H50" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E51" s="1" t="n">
         <v>4096</v>
       </c>
-      <c r="G51" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H51" s="3" t="s">
+      <c r="G51" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H51" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E52" s="1" t="n">
         <v>4096</v>
       </c>
-      <c r="G52" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H52" s="3" t="s">
+      <c r="G52" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H52" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="7" t="s">
         <v>49</v>
       </c>
       <c r="E53" s="1" t="n">
         <v>4096</v>
       </c>
-      <c r="G53" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H53" s="3" t="s">
+      <c r="G53" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H53" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="7" t="s">
         <v>50</v>
       </c>
       <c r="E54" s="1" t="n">
         <v>4096</v>
       </c>
-      <c r="G54" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H54" s="3" t="s">
+      <c r="G54" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H54" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="7" t="s">
         <v>52</v>
       </c>
       <c r="E57" s="1" t="n">
         <v>3840</v>
       </c>
-      <c r="G57" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H57" s="3" t="s">
+      <c r="G57" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H57" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="7" t="s">
         <v>53</v>
       </c>
       <c r="E58" s="1" t="n">
         <v>3840</v>
       </c>
-      <c r="G58" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H58" s="3" t="s">
+      <c r="G58" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H58" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="7" t="s">
         <v>54</v>
       </c>
       <c r="E59" s="1" t="n">
         <v>3840</v>
       </c>
-      <c r="G59" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H59" s="3" t="s">
+      <c r="G59" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H59" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="8" t="s">
+      <c r="A60" s="7" t="s">
         <v>55</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1924,179 +1927,179 @@
       <c r="E60" s="1" t="n">
         <v>3840</v>
       </c>
-      <c r="G60" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H60" s="3" t="s">
+      <c r="G60" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H60" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="8" t="s">
+      <c r="A61" s="7" t="s">
         <v>56</v>
       </c>
       <c r="E61" s="1" t="n">
         <v>3840</v>
       </c>
-      <c r="G61" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H61" s="3" t="s">
+      <c r="G61" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H61" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="8" t="s">
+      <c r="A62" s="7" t="s">
         <v>57</v>
       </c>
       <c r="E62" s="1" t="n">
         <v>3840</v>
       </c>
-      <c r="G62" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H62" s="3" t="s">
+      <c r="G62" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H62" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="8" t="s">
+      <c r="A63" s="7" t="s">
         <v>58</v>
       </c>
       <c r="E63" s="1" t="n">
         <v>3840</v>
       </c>
-      <c r="G63" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H63" s="3" t="s">
+      <c r="G63" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H63" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="8" t="s">
+      <c r="A64" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E64" s="1" t="n">
         <v>3840</v>
       </c>
-      <c r="G64" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H64" s="3" t="s">
+      <c r="G64" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H64" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="8" t="s">
+      <c r="A65" s="7" t="s">
         <v>60</v>
       </c>
       <c r="E65" s="1" t="n">
         <v>3840</v>
       </c>
-      <c r="G65" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H65" s="3" t="s">
+      <c r="G65" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H65" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="7" t="s">
         <v>62</v>
       </c>
       <c r="E68" s="1" t="n">
         <v>2048</v>
       </c>
-      <c r="G68" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H68" s="3" t="s">
+      <c r="G68" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H68" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="8" t="s">
+      <c r="A69" s="7" t="s">
         <v>63</v>
       </c>
       <c r="E69" s="1" t="n">
         <v>2048</v>
       </c>
-      <c r="G69" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H69" s="3" t="s">
+      <c r="G69" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H69" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="8" t="s">
+      <c r="A70" s="7" t="s">
         <v>64</v>
       </c>
       <c r="E70" s="1" t="n">
         <v>2048</v>
       </c>
-      <c r="G70" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H70" s="3" t="s">
+      <c r="G70" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H70" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="8" t="s">
+      <c r="A71" s="7" t="s">
         <v>65</v>
       </c>
       <c r="E71" s="1" t="n">
         <v>2048</v>
       </c>
-      <c r="G71" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H71" s="3" t="s">
+      <c r="G71" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H71" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="8" t="s">
+      <c r="A72" s="7" t="s">
         <v>66</v>
       </c>
       <c r="E72" s="1" t="n">
         <v>2048</v>
       </c>
-      <c r="G72" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H72" s="3" t="s">
+      <c r="G72" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H72" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="8" t="s">
+      <c r="A73" s="7" t="s">
         <v>67</v>
       </c>
       <c r="E73" s="1" t="n">
         <v>2048</v>
       </c>
-      <c r="G73" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H73" s="3" t="s">
+      <c r="G73" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H73" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="8" t="s">
+      <c r="A74" s="7" t="s">
         <v>68</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -2105,164 +2108,160 @@
       <c r="E74" s="1" t="n">
         <v>2048</v>
       </c>
-      <c r="G74" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H74" s="3" t="s">
+      <c r="G74" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H74" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="8" t="s">
+      <c r="A75" s="7" t="s">
         <v>70</v>
       </c>
       <c r="E75" s="1" t="n">
         <v>2048</v>
       </c>
-      <c r="G75" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H75" s="3" t="s">
+      <c r="G75" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H75" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="8" t="s">
+      <c r="A76" s="7" t="s">
         <v>71</v>
       </c>
       <c r="E76" s="1" t="n">
         <v>2048</v>
       </c>
-      <c r="G76" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H76" s="3" t="s">
+      <c r="G76" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H76" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="4" t="s">
+      <c r="A77" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="5" t="s">
+      <c r="A78" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="8" t="s">
+      <c r="A79" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C79" s="0" t="n">
         <f aca="false">LCM(E79,F79)/F79</f>
-        <v>5</v>
-      </c>
-      <c r="D79" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="D79" s="1" t="n">
         <f aca="false">LCM(E79,F79)/E79</f>
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E79" s="1" t="n">
-        <v>1920</v>
+        <v>2560</v>
       </c>
       <c r="F79" s="1" t="n">
-        <v>1152</v>
-      </c>
-      <c r="G79" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H79" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I79" s="2" t="n">
+        <v>1080</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I79" s="1" t="n">
         <f aca="false">LCM(E79,F79,G79,H79)/(F79*G79)</f>
-        <v>5</v>
-      </c>
-      <c r="J79" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="J79" s="1" t="n">
         <f aca="false">LCM(E79,F79,G79,H79)/(E79*H79)</f>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="A80" s="4"/>
       <c r="C80" s="0" t="n">
         <f aca="false">LCM(E80,F80)/F80</f>
-        <v>16</v>
-      </c>
-      <c r="D80" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="D80" s="1" t="n">
         <f aca="false">LCM(E80,F80)/E80</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E80" s="1" t="n">
-        <v>1920</v>
+        <v>2560</v>
       </c>
       <c r="F80" s="1" t="n">
         <v>1080</v>
       </c>
-      <c r="G80" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H80" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I80" s="2" t="n">
-        <f aca="false">LCM(E80*H80,F80*G80)/(F80*G80)</f>
+      <c r="G80" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H80" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J80" s="2" t="n">
-        <f aca="false">LCM(E80*H80,F80*G80)/(E80*H80)</f>
+      <c r="I80" s="1" t="n">
+        <f aca="false">LCM(E80,F80,G80,H80)/(F80*G80)</f>
+        <v>16</v>
+      </c>
+      <c r="J80" s="1" t="n">
+        <f aca="false">LCM(E80,F80,G80,H80)/(E80*H80)</f>
         <v>9</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="8"/>
-      <c r="B81" s="1" t="s">
-        <v>75</v>
+      <c r="A81" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="C81" s="0" t="n">
         <f aca="false">LCM(E81,F81)/F81</f>
-        <v>16</v>
-      </c>
-      <c r="D81" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D81" s="1" t="n">
         <f aca="false">LCM(E81,F81)/E81</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E81" s="1" t="n">
         <v>1920</v>
       </c>
       <c r="F81" s="1" t="n">
-        <v>1080</v>
-      </c>
-      <c r="G81" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H81" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I81" s="2" t="n">
-        <f aca="false">LCM(E81*H81,F81*G81)/(F81*G81)</f>
-        <v>1</v>
-      </c>
-      <c r="J81" s="2" t="n">
-        <f aca="false">LCM(E81*H81,F81*G81)/(E81*H81)</f>
-        <v>1</v>
+        <v>1152</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I81" s="1" t="n">
+        <f aca="false">LCM(E81,F81,G81,H81)/(F81*G81)</f>
+        <v>5</v>
+      </c>
+      <c r="J81" s="1" t="n">
+        <f aca="false">LCM(E81,F81,G81,H81)/(E81*H81)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="8"/>
+      <c r="A82" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="B82" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C82" s="0" t="n">
         <f aca="false">LCM(E82,F82)/F82</f>
         <v>16</v>
       </c>
-      <c r="D82" s="2" t="n">
+      <c r="D82" s="1" t="n">
         <f aca="false">LCM(E82,F82)/E82</f>
         <v>9</v>
       </c>
@@ -2272,96 +2271,99 @@
       <c r="F82" s="1" t="n">
         <v>1080</v>
       </c>
-      <c r="G82" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H82" s="3" t="s">
+      <c r="G82" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I82" s="1" t="n">
+        <f aca="false">LCM(E82*H82,F82*G82)/(F82*G82)</f>
         <v>16</v>
       </c>
-      <c r="I82" s="2" t="n">
-        <f aca="false">LCM(E82*H82,F82*G82)/(F82*G82)</f>
-        <v>4</v>
-      </c>
-      <c r="J82" s="2" t="n">
+      <c r="J82" s="1" t="n">
         <f aca="false">LCM(E82*H82,F82*G82)/(E82*H82)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="8" t="s">
+      <c r="A83" s="7"/>
+      <c r="B83" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="C83" s="0" t="n">
+        <f aca="false">LCM(E83,F83)/F83</f>
+        <v>16</v>
+      </c>
+      <c r="D83" s="1" t="n">
+        <f aca="false">LCM(E83,F83)/E83</f>
         <v>9</v>
-      </c>
-      <c r="C83" s="2" t="n">
-        <f aca="false">E83/F83</f>
-        <v>1.84971098265896</v>
-      </c>
-      <c r="D83" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="E83" s="1" t="n">
         <v>1920</v>
       </c>
       <c r="F83" s="1" t="n">
-        <v>1038</v>
-      </c>
-      <c r="G83" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H83" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I83" s="2" t="n">
+        <v>1080</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I83" s="1" t="n">
         <f aca="false">LCM(E83*H83,F83*G83)/(F83*G83)</f>
-        <v>320</v>
-      </c>
-      <c r="J83" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J83" s="1" t="n">
         <f aca="false">LCM(E83*H83,F83*G83)/(E83*H83)</f>
-        <v>173</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="8" t="s">
-        <v>77</v>
+      <c r="A84" s="7"/>
+      <c r="B84" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="C84" s="0" t="n">
         <f aca="false">LCM(E84,F84)/F84</f>
-        <v>2</v>
-      </c>
-      <c r="D84" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="D84" s="1" t="n">
         <f aca="false">LCM(E84,F84)/E84</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E84" s="1" t="n">
         <v>1920</v>
       </c>
       <c r="F84" s="1" t="n">
-        <v>960</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H84" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I84" s="2" t="n">
+        <v>1080</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I84" s="1" t="n">
         <f aca="false">LCM(E84*H84,F84*G84)/(F84*G84)</f>
-        <v>2</v>
-      </c>
-      <c r="J84" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="J84" s="1" t="n">
         <f aca="false">LCM(E84*H84,F84*G84)/(E84*H84)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C85" s="2" t="n">
+      <c r="A85" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C85" s="1" t="n">
         <f aca="false">E85/F85</f>
-        <v>2.3500611995104</v>
+        <v>1.84971098265896</v>
       </c>
       <c r="D85" s="1" t="n">
         <v>1</v>
@@ -2370,65 +2372,63 @@
         <v>1920</v>
       </c>
       <c r="F85" s="1" t="n">
-        <v>817</v>
-      </c>
-      <c r="G85" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H85" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I85" s="2" t="n">
+        <v>1038</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I85" s="1" t="n">
         <f aca="false">LCM(E85*H85,F85*G85)/(F85*G85)</f>
-        <v>1920</v>
-      </c>
-      <c r="J85" s="2" t="n">
+        <v>320</v>
+      </c>
+      <c r="J85" s="1" t="n">
         <f aca="false">LCM(E85*H85,F85*G85)/(E85*H85)</f>
-        <v>817</v>
+        <v>173</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C86" s="2" t="n">
-        <f aca="false">E86/F86</f>
-        <v>2.35294117647059</v>
+      <c r="A86" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C86" s="0" t="n">
+        <f aca="false">LCM(E86,F86)/F86</f>
+        <v>2</v>
       </c>
       <c r="D86" s="1" t="n">
+        <f aca="false">LCM(E86,F86)/E86</f>
         <v>1</v>
       </c>
       <c r="E86" s="1" t="n">
         <v>1920</v>
       </c>
       <c r="F86" s="1" t="n">
-        <v>816</v>
-      </c>
-      <c r="G86" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H86" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I86" s="2" t="n">
+        <v>960</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I86" s="1" t="n">
         <f aca="false">LCM(E86*H86,F86*G86)/(F86*G86)</f>
-        <v>40</v>
-      </c>
-      <c r="J86" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="J86" s="1" t="n">
         <f aca="false">LCM(E86*H86,F86*G86)/(E86*H86)</f>
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C87" s="2" t="n">
+      <c r="A87" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C87" s="1" t="n">
         <f aca="false">E87/F87</f>
-        <v>2.37037037037037</v>
+        <v>2.3500611995104</v>
       </c>
       <c r="D87" s="1" t="n">
         <v>1</v>
@@ -2437,31 +2437,30 @@
         <v>1920</v>
       </c>
       <c r="F87" s="1" t="n">
-        <v>810</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H87" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I87" s="2" t="n">
+        <v>817</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I87" s="1" t="n">
         <f aca="false">LCM(E87*H87,F87*G87)/(F87*G87)</f>
-        <v>64</v>
-      </c>
-      <c r="J87" s="2" t="n">
+        <v>1920</v>
+      </c>
+      <c r="J87" s="1" t="n">
         <f aca="false">LCM(E87*H87,F87*G87)/(E87*H87)</f>
-        <v>27</v>
+        <v>817</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="8"/>
-      <c r="B88" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C88" s="2" t="n">
+      <c r="A88" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C88" s="1" t="n">
         <f aca="false">E88/F88</f>
-        <v>2.37037037037037</v>
+        <v>2.35294117647059</v>
       </c>
       <c r="D88" s="1" t="n">
         <v>1</v>
@@ -2470,29 +2469,31 @@
         <v>1920</v>
       </c>
       <c r="F88" s="1" t="n">
-        <v>810</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H88" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I88" s="2" t="n">
+        <v>816</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I88" s="1" t="n">
         <f aca="false">LCM(E88*H88,F88*G88)/(F88*G88)</f>
-        <v>4</v>
-      </c>
-      <c r="J88" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="J88" s="1" t="n">
         <f aca="false">LCM(E88*H88,F88*G88)/(E88*H88)</f>
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="8"/>
+      <c r="A89" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="B89" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C89" s="2" t="n">
+      <c r="C89" s="1" t="n">
         <f aca="false">E89/F89</f>
         <v>2.37037037037037</v>
       </c>
@@ -2505,28 +2506,29 @@
       <c r="F89" s="1" t="n">
         <v>810</v>
       </c>
-      <c r="G89" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I89" s="2" t="n">
+      <c r="G89" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I89" s="1" t="n">
         <f aca="false">LCM(E89*H89,F89*G89)/(F89*G89)</f>
-        <v>16</v>
-      </c>
-      <c r="J89" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="J89" s="1" t="n">
         <f aca="false">LCM(E89*H89,F89*G89)/(E89*H89)</f>
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C90" s="2" t="n">
+      <c r="A90" s="7"/>
+      <c r="B90" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C90" s="1" t="n">
         <f aca="false">E90/F90</f>
-        <v>2.39103362391034</v>
+        <v>2.37037037037037</v>
       </c>
       <c r="D90" s="1" t="n">
         <v>1</v>
@@ -2535,33 +2537,31 @@
         <v>1920</v>
       </c>
       <c r="F90" s="1" t="n">
-        <v>803</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H90" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I90" s="2" t="n">
+        <v>810</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I90" s="1" t="n">
         <f aca="false">LCM(E90*H90,F90*G90)/(F90*G90)</f>
-        <v>1920</v>
-      </c>
-      <c r="J90" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="J90" s="1" t="n">
         <f aca="false">LCM(E90*H90,F90*G90)/(E90*H90)</f>
-        <v>803</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="8" t="s">
-        <v>82</v>
-      </c>
+      <c r="A91" s="7"/>
       <c r="B91" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C91" s="2" t="n">
+        <v>69</v>
+      </c>
+      <c r="C91" s="1" t="n">
         <f aca="false">E91/F91</f>
-        <v>2.4</v>
+        <v>2.37037037037037</v>
       </c>
       <c r="D91" s="1" t="n">
         <v>1</v>
@@ -2570,198 +2570,203 @@
         <v>1920</v>
       </c>
       <c r="F91" s="1" t="n">
+        <v>810</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I91" s="1" t="n">
+        <f aca="false">LCM(E91*H91,F91*G91)/(F91*G91)</f>
+        <v>16</v>
+      </c>
+      <c r="J91" s="1" t="n">
+        <f aca="false">LCM(E91*H91,F91*G91)/(E91*H91)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C92" s="1" t="n">
+        <f aca="false">E92/F92</f>
+        <v>2.39103362391034</v>
+      </c>
+      <c r="D92" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E92" s="1" t="n">
+        <v>1920</v>
+      </c>
+      <c r="F92" s="1" t="n">
+        <v>803</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I92" s="1" t="n">
+        <f aca="false">LCM(E92*H92,F92*G92)/(F92*G92)</f>
+        <v>1920</v>
+      </c>
+      <c r="J92" s="1" t="n">
+        <f aca="false">LCM(E92*H92,F92*G92)/(E92*H92)</f>
+        <v>803</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C93" s="1" t="n">
+        <f aca="false">E93/F93</f>
+        <v>2.4</v>
+      </c>
+      <c r="D93" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E93" s="1" t="n">
+        <v>1920</v>
+      </c>
+      <c r="F93" s="1" t="n">
         <v>800</v>
       </c>
-      <c r="G91" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H91" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I91" s="2" t="n">
-        <f aca="false">LCM(E91*H91,F91*G91)/(F91*G91)</f>
+      <c r="G93" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I93" s="1" t="n">
+        <f aca="false">LCM(E93*H93,F93*G93)/(F93*G93)</f>
         <v>12</v>
       </c>
-      <c r="J91" s="2" t="n">
-        <f aca="false">LCM(E91*H91,F91*G91)/(E91*H91)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="8"/>
-      <c r="B92" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C92" s="2" t="n">
-        <f aca="false">C91</f>
-        <v>2.4</v>
-      </c>
-      <c r="D92" s="2" t="n">
-        <f aca="false">D91</f>
-        <v>1</v>
-      </c>
-      <c r="E92" s="2" t="n">
-        <f aca="false">E91</f>
-        <v>1920</v>
-      </c>
-      <c r="F92" s="2" t="n">
-        <f aca="false">F91</f>
-        <v>800</v>
-      </c>
-      <c r="G92" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H92" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I92" s="2" t="n">
-        <f aca="false">LCM(E92*H92,F92*G92)/(F92*G92)</f>
-        <v>27</v>
-      </c>
-      <c r="J92" s="2" t="n">
-        <f aca="false">LCM(E92*H92,F92*G92)/(E92*H92)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="8"/>
-      <c r="B93" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C93" s="2" t="n">
-        <f aca="false">C92</f>
-        <v>2.4</v>
-      </c>
-      <c r="D93" s="2" t="n">
-        <f aca="false">D92</f>
-        <v>1</v>
-      </c>
-      <c r="E93" s="2" t="n">
-        <f aca="false">E92</f>
-        <v>1920</v>
-      </c>
-      <c r="F93" s="2" t="n">
-        <f aca="false">F92</f>
-        <v>800</v>
-      </c>
-      <c r="G93" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H93" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I93" s="2" t="n">
-        <f aca="false">LCM(E93*H93,F93*G93)/(F93*G93)</f>
-        <v>9</v>
-      </c>
-      <c r="J93" s="2" t="n">
+      <c r="J93" s="1" t="n">
         <f aca="false">LCM(E93*H93,F93*G93)/(E93*H93)</f>
         <v>5</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="8" t="s">
+      <c r="A94" s="7"/>
+      <c r="B94" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C94" s="2" t="n">
-        <f aca="false">E94/F94</f>
+      <c r="C94" s="1" t="n">
+        <f aca="false">C93</f>
+        <v>2.4</v>
+      </c>
+      <c r="D94" s="1" t="n">
+        <f aca="false">D93</f>
+        <v>1</v>
+      </c>
+      <c r="E94" s="1" t="n">
+        <f aca="false">E93</f>
+        <v>1920</v>
+      </c>
+      <c r="F94" s="1" t="n">
+        <f aca="false">F93</f>
+        <v>800</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I94" s="1" t="n">
+        <f aca="false">LCM(E94*H94,F94*G94)/(F94*G94)</f>
+        <v>27</v>
+      </c>
+      <c r="J94" s="1" t="n">
+        <f aca="false">LCM(E94*H94,F94*G94)/(E94*H94)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="7"/>
+      <c r="B95" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C95" s="1" t="n">
+        <f aca="false">C94</f>
+        <v>2.4</v>
+      </c>
+      <c r="D95" s="1" t="n">
+        <f aca="false">D94</f>
+        <v>1</v>
+      </c>
+      <c r="E95" s="1" t="n">
+        <f aca="false">E94</f>
+        <v>1920</v>
+      </c>
+      <c r="F95" s="1" t="n">
+        <f aca="false">F94</f>
+        <v>800</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I95" s="1" t="n">
+        <f aca="false">LCM(E95*H95,F95*G95)/(F95*G95)</f>
+        <v>9</v>
+      </c>
+      <c r="J95" s="1" t="n">
+        <f aca="false">LCM(E95*H95,F95*G95)/(E95*H95)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C96" s="1" t="n">
+        <f aca="false">E96/F96</f>
         <v>2.43964421855146</v>
       </c>
-      <c r="D94" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E94" s="1" t="n">
-        <v>1920</v>
-      </c>
-      <c r="F94" s="1" t="n">
-        <v>787</v>
-      </c>
-      <c r="G94" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H94" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I94" s="2" t="n">
-        <f aca="false">LCM(E94*H94,F94*G94)/(F94*G94)</f>
-        <v>1920</v>
-      </c>
-      <c r="J94" s="2" t="n">
-        <f aca="false">LCM(E94*H94,F94*G94)/(E94*H94)</f>
-        <v>787</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C95" s="0" t="n">
-        <f aca="false">LCM(E95,F95)/F95</f>
-        <v>4</v>
-      </c>
-      <c r="D95" s="2" t="n">
-        <f aca="false">LCM(E95,F95)/E95</f>
-        <v>3</v>
-      </c>
-      <c r="E95" s="1" t="n">
-        <v>1920</v>
-      </c>
-      <c r="F95" s="1" t="n">
-        <v>1440</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H95" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I95" s="2" t="n">
-        <f aca="false">LCM(E95*H95,F95*G95)/(F95*G95)</f>
-        <v>4</v>
-      </c>
-      <c r="J95" s="2" t="n">
-        <f aca="false">LCM(E95*H95,F95*G95)/(E95*H95)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="8"/>
-      <c r="C96" s="0" t="n">
-        <f aca="false">LCM(E96,F96)/F96</f>
-        <v>4</v>
-      </c>
-      <c r="D96" s="2" t="n">
-        <f aca="false">LCM(E96,F96)/E96</f>
-        <v>3</v>
+      <c r="D96" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="E96" s="1" t="n">
         <v>1920</v>
       </c>
       <c r="F96" s="1" t="n">
-        <v>1440</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H96" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I96" s="2" t="n">
+        <v>787</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I96" s="1" t="n">
         <f aca="false">LCM(E96*H96,F96*G96)/(F96*G96)</f>
-        <v>1</v>
-      </c>
-      <c r="J96" s="2" t="n">
+        <v>1920</v>
+      </c>
+      <c r="J96" s="1" t="n">
         <f aca="false">LCM(E96*H96,F96*G96)/(E96*H96)</f>
-        <v>1</v>
+        <v>787</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="8"/>
+      <c r="A97" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="C97" s="0" t="n">
         <f aca="false">LCM(E97,F97)/F97</f>
         <v>4</v>
       </c>
-      <c r="D97" s="2" t="n">
+      <c r="D97" s="1" t="n">
         <f aca="false">LCM(E97,F97)/E97</f>
         <v>3</v>
       </c>
@@ -2771,276 +2776,276 @@
       <c r="F97" s="1" t="n">
         <v>1440</v>
       </c>
-      <c r="G97" s="3" t="s">
+      <c r="G97" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I97" s="1" t="n">
+        <f aca="false">LCM(E97*H97,F97*G97)/(F97*G97)</f>
+        <v>4</v>
+      </c>
+      <c r="J97" s="1" t="n">
+        <f aca="false">LCM(E97*H97,F97*G97)/(E97*H97)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="7"/>
+      <c r="C98" s="0" t="n">
+        <f aca="false">LCM(E98,F98)/F98</f>
+        <v>4</v>
+      </c>
+      <c r="D98" s="1" t="n">
+        <f aca="false">LCM(E98,F98)/E98</f>
+        <v>3</v>
+      </c>
+      <c r="E98" s="1" t="n">
+        <v>1920</v>
+      </c>
+      <c r="F98" s="1" t="n">
+        <v>1440</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I98" s="1" t="n">
+        <f aca="false">LCM(E98*H98,F98*G98)/(F98*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="J98" s="1" t="n">
+        <f aca="false">LCM(E98*H98,F98*G98)/(E98*H98)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="7"/>
+      <c r="C99" s="0" t="n">
+        <f aca="false">LCM(E99,F99)/F99</f>
+        <v>4</v>
+      </c>
+      <c r="D99" s="1" t="n">
+        <f aca="false">LCM(E99,F99)/E99</f>
+        <v>3</v>
+      </c>
+      <c r="E99" s="1" t="n">
+        <v>1920</v>
+      </c>
+      <c r="F99" s="1" t="n">
+        <v>1440</v>
+      </c>
+      <c r="G99" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H97" s="3" t="s">
+      <c r="H99" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I97" s="2" t="n">
-        <f aca="false">LCM(E97*H97,F97*G97)/(F97*G97)</f>
+      <c r="I99" s="1" t="n">
+        <f aca="false">LCM(E99*H99,F99*G99)/(F99*G99)</f>
         <v>3</v>
       </c>
-      <c r="J97" s="2" t="n">
-        <f aca="false">LCM(E97*H97,F97*G97)/(E97*H97)</f>
+      <c r="J99" s="1" t="n">
+        <f aca="false">LCM(E99*H99,F99*G99)/(E99*H99)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="8"/>
-      <c r="C98" s="0"/>
-      <c r="D98" s="2"/>
-    </row>
-    <row r="99" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="8" t="s">
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="7"/>
+      <c r="C100" s="0"/>
+    </row>
+    <row r="101" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C101" s="0" t="n">
-        <f aca="false">LCM(E101,F101)/F101</f>
-        <v>4</v>
-      </c>
-      <c r="D101" s="2" t="n">
-        <f aca="false">LCM(E101,F101)/E101</f>
-        <v>3</v>
-      </c>
-      <c r="E101" s="1" t="n">
-        <v>1280</v>
-      </c>
-      <c r="F101" s="1" t="n">
-        <v>960</v>
-      </c>
-      <c r="G101" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H101" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I101" s="2" t="n">
-        <f aca="false">LCM(E101*H101,F101*G101)/(F101*G101)</f>
-        <v>4</v>
-      </c>
-      <c r="J101" s="2" t="n">
-        <f aca="false">LCM(E101*H101,F101*G101)/(E101*H101)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="8" t="s">
+    </row>
+    <row r="102" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="C102" s="0" t="n">
-        <f aca="false">LCM(E102,F102)/F102</f>
-        <v>5</v>
-      </c>
-      <c r="D102" s="2" t="n">
-        <f aca="false">LCM(E102,F102)/E102</f>
-        <v>3</v>
-      </c>
-      <c r="E102" s="1" t="n">
-        <v>1280</v>
-      </c>
-      <c r="F102" s="1" t="n">
-        <v>768</v>
-      </c>
-      <c r="G102" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H102" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I102" s="2" t="n">
-        <f aca="false">LCM(E102*H102,F102*G102)/(F102*G102)</f>
-        <v>5</v>
-      </c>
-      <c r="J102" s="2" t="n">
-        <f aca="false">LCM(E102*H102,F102*G102)/(E102*H102)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="C103" s="0" t="n">
         <f aca="false">LCM(E103,F103)/F103</f>
-        <v>16</v>
-      </c>
-      <c r="D103" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D103" s="1" t="n">
         <f aca="false">LCM(E103,F103)/E103</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E103" s="1" t="n">
         <v>1280</v>
       </c>
       <c r="F103" s="1" t="n">
-        <v>720</v>
-      </c>
-      <c r="G103" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H103" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I103" s="2" t="n">
+        <v>960</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I103" s="1" t="n">
         <f aca="false">LCM(E103*H103,F103*G103)/(F103*G103)</f>
-        <v>16</v>
-      </c>
-      <c r="J103" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="J103" s="1" t="n">
         <f aca="false">LCM(E103*H103,F103*G103)/(E103*H103)</f>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C104" s="2" t="n">
-        <f aca="false">E104/F104</f>
-        <v>1.84971098265896</v>
+      <c r="A104" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C104" s="0" t="n">
+        <f aca="false">LCM(E104,F104)/F104</f>
+        <v>5</v>
       </c>
       <c r="D104" s="1" t="n">
-        <v>1</v>
+        <f aca="false">LCM(E104,F104)/E104</f>
+        <v>3</v>
       </c>
       <c r="E104" s="1" t="n">
         <v>1280</v>
       </c>
       <c r="F104" s="1" t="n">
-        <v>692</v>
-      </c>
-      <c r="G104" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H104" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I104" s="2" t="n">
+        <v>768</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I104" s="1" t="n">
         <f aca="false">LCM(E104*H104,F104*G104)/(F104*G104)</f>
-        <v>320</v>
-      </c>
-      <c r="J104" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J104" s="1" t="n">
         <f aca="false">LCM(E104*H104,F104*G104)/(E104*H104)</f>
-        <v>173</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C105" s="2" t="n">
-        <f aca="false">E105/F105</f>
-        <v>2</v>
+      <c r="A105" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C105" s="0" t="n">
+        <f aca="false">LCM(E105,F105)/F105</f>
+        <v>16</v>
       </c>
       <c r="D105" s="1" t="n">
-        <v>1</v>
+        <f aca="false">LCM(E105,F105)/E105</f>
+        <v>9</v>
       </c>
       <c r="E105" s="1" t="n">
         <v>1280</v>
       </c>
       <c r="F105" s="1" t="n">
-        <v>640</v>
-      </c>
-      <c r="G105" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H105" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I105" s="2" t="n">
+        <v>720</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I105" s="1" t="n">
         <f aca="false">LCM(E105*H105,F105*G105)/(F105*G105)</f>
-        <v>2</v>
-      </c>
-      <c r="J105" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="J105" s="1" t="n">
         <f aca="false">LCM(E105*H105,F105*G105)/(E105*H105)</f>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C106" s="2" t="n">
-        <f aca="false">E106/F106</f>
-        <v>2.34862385321101</v>
+      <c r="A106" s="7"/>
+      <c r="B106" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C106" s="0" t="n">
+        <f aca="false">LCM(E106,F106)/F106</f>
+        <v>16</v>
       </c>
       <c r="D106" s="1" t="n">
-        <v>1</v>
+        <f aca="false">LCM(E106,F106)/E106</f>
+        <v>9</v>
       </c>
       <c r="E106" s="1" t="n">
         <v>1280</v>
       </c>
       <c r="F106" s="1" t="n">
-        <v>545</v>
-      </c>
-      <c r="G106" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H106" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I106" s="2" t="n">
+        <v>720</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I106" s="1" t="n">
         <f aca="false">LCM(E106*H106,F106*G106)/(F106*G106)</f>
-        <v>256</v>
-      </c>
-      <c r="J106" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="J106" s="1" t="n">
         <f aca="false">LCM(E106*H106,F106*G106)/(E106*H106)</f>
-        <v>109</v>
+        <v>3</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C107" s="2" t="n">
-        <f aca="false">E107/F107</f>
-        <v>2.37037037037037</v>
+      <c r="A107" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C107" s="0" t="n">
+        <f aca="false">LCM(E107,F107)/F107</f>
+        <v>7</v>
       </c>
       <c r="D107" s="1" t="n">
-        <v>1</v>
+        <f aca="false">LCM(E107,F107)/E107</f>
+        <v>3</v>
       </c>
       <c r="E107" s="1" t="n">
-        <v>1280</v>
+        <v>1680</v>
       </c>
       <c r="F107" s="1" t="n">
-        <v>540</v>
-      </c>
-      <c r="G107" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H107" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I107" s="2" t="n">
+        <v>720</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I107" s="1" t="n">
         <f aca="false">LCM(E107*H107,F107*G107)/(F107*G107)</f>
-        <v>64</v>
-      </c>
-      <c r="J107" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="J107" s="1" t="n">
         <f aca="false">LCM(E107*H107,F107*G107)/(E107*H107)</f>
-        <v>27</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C108" s="2" t="n">
+      <c r="A108" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C108" s="1" t="n">
         <f aca="false">E108/F108</f>
-        <v>2.38805970149254</v>
+        <v>1.84971098265896</v>
       </c>
       <c r="D108" s="1" t="n">
         <v>1</v>
@@ -3049,30 +3054,30 @@
         <v>1280</v>
       </c>
       <c r="F108" s="1" t="n">
-        <v>536</v>
-      </c>
-      <c r="G108" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H108" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I108" s="2" t="n">
+        <v>692</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I108" s="1" t="n">
         <f aca="false">LCM(E108*H108,F108*G108)/(F108*G108)</f>
-        <v>160</v>
-      </c>
-      <c r="J108" s="2" t="n">
+        <v>320</v>
+      </c>
+      <c r="J108" s="1" t="n">
         <f aca="false">LCM(E108*H108,F108*G108)/(E108*H108)</f>
-        <v>67</v>
+        <v>173</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C109" s="2" t="n">
+      <c r="A109" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C109" s="1" t="n">
         <f aca="false">E109/F109</f>
-        <v>2.43809523809524</v>
+        <v>2</v>
       </c>
       <c r="D109" s="1" t="n">
         <v>1</v>
@@ -3081,21 +3086,155 @@
         <v>1280</v>
       </c>
       <c r="F109" s="1" t="n">
+        <v>640</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I109" s="1" t="n">
+        <f aca="false">LCM(E109*H109,F109*G109)/(F109*G109)</f>
+        <v>2</v>
+      </c>
+      <c r="J109" s="1" t="n">
+        <f aca="false">LCM(E109*H109,F109*G109)/(E109*H109)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C110" s="1" t="n">
+        <f aca="false">E110/F110</f>
+        <v>2.34862385321101</v>
+      </c>
+      <c r="D110" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E110" s="1" t="n">
+        <v>1280</v>
+      </c>
+      <c r="F110" s="1" t="n">
+        <v>545</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I110" s="1" t="n">
+        <f aca="false">LCM(E110*H110,F110*G110)/(F110*G110)</f>
+        <v>256</v>
+      </c>
+      <c r="J110" s="1" t="n">
+        <f aca="false">LCM(E110*H110,F110*G110)/(E110*H110)</f>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C111" s="1" t="n">
+        <f aca="false">E111/F111</f>
+        <v>2.37037037037037</v>
+      </c>
+      <c r="D111" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E111" s="1" t="n">
+        <v>1280</v>
+      </c>
+      <c r="F111" s="1" t="n">
+        <v>540</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I111" s="1" t="n">
+        <f aca="false">LCM(E111*H111,F111*G111)/(F111*G111)</f>
+        <v>64</v>
+      </c>
+      <c r="J111" s="1" t="n">
+        <f aca="false">LCM(E111*H111,F111*G111)/(E111*H111)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C112" s="1" t="n">
+        <f aca="false">E112/F112</f>
+        <v>2.38805970149254</v>
+      </c>
+      <c r="D112" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E112" s="1" t="n">
+        <v>1280</v>
+      </c>
+      <c r="F112" s="1" t="n">
+        <v>536</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I112" s="1" t="n">
+        <f aca="false">LCM(E112*H112,F112*G112)/(F112*G112)</f>
+        <v>160</v>
+      </c>
+      <c r="J112" s="1" t="n">
+        <f aca="false">LCM(E112*H112,F112*G112)/(E112*H112)</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C113" s="1" t="n">
+        <f aca="false">E113/F113</f>
+        <v>2.43809523809524</v>
+      </c>
+      <c r="D113" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E113" s="1" t="n">
+        <v>1280</v>
+      </c>
+      <c r="F113" s="1" t="n">
         <v>525</v>
       </c>
-      <c r="G109" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H109" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I109" s="2" t="n">
-        <f aca="false">LCM(E109*H109,F109*G109)/(F109*G109)</f>
+      <c r="G113" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H113" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I113" s="1" t="n">
+        <f aca="false">LCM(E113*H113,F113*G113)/(F113*G113)</f>
         <v>256</v>
       </c>
-      <c r="J109" s="2" t="n">
-        <f aca="false">LCM(E109*H109,F109*G109)/(E109*H109)</f>
+      <c r="J113" s="1" t="n">
+        <f aca="false">LCM(E113*H113,F113*G113)/(E113*H113)</f>
         <v>105</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D114" s="1" t="n">
+        <f aca="false">9/21*1280</f>
+        <v>548.571428571429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update spreadsheet, add 35mm infographic
</commit_message>
<xml_diff>
--- a/display-pixel-ratios.xlsx
+++ b/display-pixel-ratios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulyc/development/provideotoolbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D5CEBC-1344-214D-8531-8D33446D5C9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAED7AB-4A4A-D44B-8B30-B4767E471020}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10400" yWindow="8820" windowWidth="24780" windowHeight="17160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9360" yWindow="8780" windowWidth="24780" windowHeight="17160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="110">
   <si>
     <t>CINEMA DCP 4k</t>
   </si>
@@ -273,9 +273,6 @@
     <t>2.39:1 (referred to as 2.40)  /  1920x803</t>
   </si>
   <si>
-    <t>2.40:1 (Blu-Ray)  /  1920x800</t>
-  </si>
-  <si>
     <t>Blu-Ray</t>
   </si>
   <si>
@@ -346,6 +343,18 @@
   </si>
   <si>
     <t>FAR:1</t>
+  </si>
+  <si>
+    <t>2.40:1 (Blu-Ray Cropped)  /  1920x800</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>??? UHD Rip</t>
   </si>
 </sst>
 </file>
@@ -494,12 +503,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -519,6 +522,12 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -834,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L124"/>
+  <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -860,7 +869,7 @@
     </row>
     <row r="2" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -872,43 +881,43 @@
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
     </row>
-    <row r="3" spans="1:10" s="29" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" s="21" t="s">
+    <row r="3" spans="1:10" s="27" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="25"/>
+      <c r="B3" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="28" t="s">
+      <c r="D3" s="29"/>
+      <c r="E3" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="F3" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21" t="s">
+      <c r="G3" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="21"/>
-    </row>
-    <row r="4" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
-        <v>98</v>
+      <c r="J3" s="29"/>
+    </row>
+    <row r="4" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>97</v>
       </c>
       <c r="B4" s="14">
         <f>C4/D4</f>
         <v>1.375</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="21">
         <f>I4</f>
         <v>11</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="21">
         <f>J4</f>
         <v>8</v>
       </c>
@@ -926,25 +935,25 @@
         <f>LCM(C4*J4,D4*I4)/(C4*J4)</f>
         <v>1</v>
       </c>
-      <c r="I4" s="24">
+      <c r="I4" s="22">
         <v>11</v>
       </c>
-      <c r="J4" s="24">
+      <c r="J4" s="22">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
-        <v>100</v>
+    <row r="5" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="24" t="s">
+        <v>99</v>
       </c>
       <c r="B5" s="14">
         <f>C5/D5</f>
         <v>1.7777777777777777</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="21">
         <v>16</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="21">
         <v>9</v>
       </c>
       <c r="E5" s="14">
@@ -970,17 +979,17 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
-        <v>104</v>
+      <c r="A6" s="20" t="s">
+        <v>103</v>
       </c>
       <c r="B6" s="14">
         <f>C6/D6</f>
         <v>2.3468531468531468</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="22">
         <v>1678</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="22">
         <v>715</v>
       </c>
       <c r="E6" s="14">
@@ -1004,18 +1013,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
-        <v>105</v>
+    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>104</v>
       </c>
       <c r="B7" s="14">
         <f>C7/D7</f>
         <v>2.3869463869463869</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="22">
         <v>1024</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="22">
         <v>429</v>
       </c>
       <c r="E7" s="14">
@@ -1032,24 +1041,24 @@
         <f>LCM(C7*J7,D7*I7)/(C7*J7)</f>
         <v>4719</v>
       </c>
-      <c r="I7" s="24">
+      <c r="I7" s="22">
         <v>11</v>
       </c>
-      <c r="J7" s="24">
+      <c r="J7" s="22">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:10" s="13" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
@@ -1067,32 +1076,32 @@
     </row>
     <row r="10" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="20"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="14" t="s">
         <v>3</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="21"/>
-      <c r="I10" s="20" t="s">
+      <c r="H10" s="29"/>
+      <c r="I10" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="20"/>
+      <c r="J10" s="28"/>
     </row>
     <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="20" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="14" t="s">
@@ -1118,7 +1127,7 @@
         <v>9</v>
       </c>
       <c r="I11" s="14">
-        <f t="shared" ref="G11:I20" si="0">LCM(E11*H11,F11*G11)/(F11*G11)</f>
+        <f t="shared" ref="I11:I20" si="0">LCM(E11*H11,F11*G11)/(F11*G11)</f>
         <v>37</v>
       </c>
       <c r="J11" s="14">
@@ -1127,7 +1136,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="22"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="14" t="s">
         <v>8</v>
       </c>
@@ -1159,7 +1168,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="20" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="14" t="s">
@@ -1194,7 +1203,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="22"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="14" t="s">
         <v>11</v>
       </c>
@@ -1229,7 +1238,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="22"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="14" t="s">
         <v>11</v>
       </c>
@@ -1264,7 +1273,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="22"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="14" t="s">
         <v>11</v>
       </c>
@@ -1294,7 +1303,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="20" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="14" t="s">
@@ -1330,7 +1339,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="20" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="14" t="s">
@@ -1365,7 +1374,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="22"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="14" t="s">
         <v>19</v>
       </c>
@@ -1400,7 +1409,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="22"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="14" t="s">
         <v>19</v>
       </c>
@@ -1434,7 +1443,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="22"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="14" t="s">
         <v>19</v>
       </c>
@@ -1479,7 +1488,7 @@
     </row>
     <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -1492,7 +1501,7 @@
       <c r="J23" s="14"/>
     </row>
     <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="14" t="s">
@@ -1527,7 +1536,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="20" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="14" t="s">
@@ -1562,7 +1571,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="22"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="14" t="s">
         <v>11</v>
       </c>
@@ -1595,7 +1604,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="22"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="14" t="s">
         <v>11</v>
       </c>
@@ -1628,7 +1637,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="14" t="s">
@@ -1664,7 +1673,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="20" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="14" t="s">
@@ -1699,7 +1708,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="22"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="14" t="s">
         <v>19</v>
       </c>
@@ -1732,7 +1741,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="22"/>
+      <c r="A31" s="20"/>
       <c r="B31" s="14" t="s">
         <v>19</v>
       </c>
@@ -1780,7 +1789,7 @@
     </row>
     <row r="33" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -1793,7 +1802,7 @@
       <c r="J33" s="14"/>
     </row>
     <row r="34" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="20" t="s">
         <v>26</v>
       </c>
       <c r="B34" s="14"/>
@@ -1827,7 +1836,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="22" t="s">
+      <c r="A35" s="20" t="s">
         <v>27</v>
       </c>
       <c r="B35" s="14"/>
@@ -1861,7 +1870,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="22" t="s">
+      <c r="A36" s="20" t="s">
         <v>28</v>
       </c>
       <c r="B36" s="14"/>
@@ -1895,7 +1904,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="20" t="s">
         <v>29</v>
       </c>
       <c r="B37" s="14" t="s">
@@ -1930,7 +1939,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="22" t="s">
+      <c r="A38" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B38" s="14" t="s">
@@ -1965,7 +1974,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="22"/>
+      <c r="A39" s="20"/>
       <c r="B39" s="14" t="s">
         <v>19</v>
       </c>
@@ -1998,7 +2007,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="22"/>
+      <c r="A40" s="20"/>
       <c r="B40" s="14" t="s">
         <v>19</v>
       </c>
@@ -2031,7 +2040,7 @@
       </c>
     </row>
     <row r="41" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="22" t="s">
+      <c r="A41" s="20" t="s">
         <v>31</v>
       </c>
       <c r="B41" s="14"/>
@@ -2064,8 +2073,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A42" s="22" t="s">
+    <row r="42" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B42" s="14" t="s">
@@ -2100,7 +2109,7 @@
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="22"/>
+      <c r="A43" s="20"/>
       <c r="B43" s="14" t="s">
         <v>33</v>
       </c>
@@ -2133,7 +2142,7 @@
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="22"/>
+      <c r="A44" s="20"/>
       <c r="B44" s="14" t="s">
         <v>33</v>
       </c>
@@ -2165,8 +2174,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A45" s="22" t="s">
+    <row r="45" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B45" s="14"/>
@@ -2200,7 +2209,7 @@
       <c r="L45" s="11"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="22"/>
+      <c r="A46" s="20"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14">
         <f t="shared" si="6"/>
@@ -2231,7 +2240,7 @@
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A47" s="22"/>
+      <c r="A47" s="20"/>
       <c r="B47" s="14"/>
       <c r="C47" s="14">
         <f t="shared" si="6"/>
@@ -2262,7 +2271,7 @@
       </c>
     </row>
     <row r="48" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="22" t="s">
+      <c r="A48" s="20" t="s">
         <v>35</v>
       </c>
       <c r="B48" s="14"/>
@@ -2295,7 +2304,7 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" s="22"/>
+      <c r="A49" s="20"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14">
         <f t="shared" si="6"/>
@@ -2326,7 +2335,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="22" t="s">
+      <c r="A50" s="20" t="s">
         <v>36</v>
       </c>
       <c r="B50" s="14"/>
@@ -2359,10 +2368,10 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="22" t="s">
+      <c r="A51" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B51" s="23"/>
+      <c r="B51" s="21"/>
       <c r="C51" s="14">
         <f t="shared" si="6"/>
         <v>2.3497016980266179</v>
@@ -2392,10 +2401,10 @@
       </c>
     </row>
     <row r="52" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="22" t="s">
+      <c r="A52" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B52" s="23"/>
+      <c r="B52" s="21"/>
       <c r="C52" s="14">
         <f t="shared" si="6"/>
         <v>2.3486238532110093</v>
@@ -2440,7 +2449,7 @@
     </row>
     <row r="54" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
@@ -2453,7 +2462,7 @@
       <c r="J54" s="14"/>
     </row>
     <row r="55" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="22" t="s">
+      <c r="A55" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B55" s="14"/>
@@ -2485,7 +2494,7 @@
       </c>
     </row>
     <row r="56" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="22" t="s">
+      <c r="A56" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B56" s="14"/>
@@ -2517,7 +2526,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="22" t="s">
+      <c r="A57" s="20" t="s">
         <v>42</v>
       </c>
       <c r="B57" s="14"/>
@@ -2549,14 +2558,14 @@
       </c>
     </row>
     <row r="58" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="22" t="s">
+      <c r="A58" s="20" t="s">
         <v>43</v>
       </c>
       <c r="B58" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C58" s="14">
-        <f t="shared" ref="C55:C64" si="9">E58/F58</f>
+        <f t="shared" ref="C58:C64" si="9">E58/F58</f>
         <v>1.8500451671183378</v>
       </c>
       <c r="D58" s="14">
@@ -2583,8 +2592,8 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A59" s="22" t="s">
+    <row r="59" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="20" t="s">
         <v>44</v>
       </c>
       <c r="B59" s="14"/>
@@ -2617,7 +2626,7 @@
       </c>
     </row>
     <row r="60" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="22" t="s">
+      <c r="A60" s="20" t="s">
         <v>45</v>
       </c>
       <c r="B60" s="14"/>
@@ -2650,7 +2659,7 @@
       </c>
     </row>
     <row r="61" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="22" t="s">
+      <c r="A61" s="20" t="s">
         <v>46</v>
       </c>
       <c r="B61" s="14"/>
@@ -2683,7 +2692,7 @@
       </c>
     </row>
     <row r="62" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="22" t="s">
+      <c r="A62" s="20" t="s">
         <v>47</v>
       </c>
       <c r="B62" s="14"/>
@@ -2715,8 +2724,8 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A63" s="22" t="s">
+    <row r="63" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="20" t="s">
         <v>48</v>
       </c>
       <c r="B63" s="14"/>
@@ -2749,7 +2758,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="22" t="s">
+      <c r="A64" s="20" t="s">
         <v>49</v>
       </c>
       <c r="B64" s="14"/>
@@ -2797,7 +2806,7 @@
     </row>
     <row r="66" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B66" s="14"/>
       <c r="C66" s="14"/>
@@ -2810,7 +2819,7 @@
       <c r="J66" s="14"/>
     </row>
     <row r="67" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="22" t="s">
+      <c r="A67" s="20" t="s">
         <v>51</v>
       </c>
       <c r="B67" s="14"/>
@@ -2833,16 +2842,16 @@
         <v>9</v>
       </c>
       <c r="I67" s="14">
-        <f t="shared" ref="I67:I75" si="10">LCM(E67*H67,F67*G67)/(F67*G67)</f>
+        <f t="shared" ref="I67:I74" si="10">LCM(E67*H67,F67*G67)/(F67*G67)</f>
         <v>4</v>
       </c>
       <c r="J67" s="14">
-        <f t="shared" ref="J67:J75" si="11">LCM(E67*H67,F67*G67)/(E67*H67)</f>
+        <f t="shared" ref="J67:J74" si="11">LCM(E67*H67,F67*G67)/(E67*H67)</f>
         <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="22" t="s">
+      <c r="A68" s="20" t="s">
         <v>52</v>
       </c>
       <c r="B68" s="14"/>
@@ -2874,7 +2883,7 @@
       </c>
     </row>
     <row r="69" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="22" t="s">
+      <c r="A69" s="20" t="s">
         <v>53</v>
       </c>
       <c r="B69" s="14"/>
@@ -2906,14 +2915,14 @@
       </c>
     </row>
     <row r="70" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="22" t="s">
+      <c r="A70" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B70" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C70" s="14">
-        <f t="shared" ref="C67:C75" si="12">E70/F70</f>
+        <f t="shared" ref="C70:C74" si="12">E70/F70</f>
         <v>1.8497109826589595</v>
       </c>
       <c r="D70" s="14">
@@ -2941,7 +2950,7 @@
       </c>
     </row>
     <row r="71" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="22" t="s">
+      <c r="A71" s="20" t="s">
         <v>55</v>
       </c>
       <c r="B71" s="14"/>
@@ -2974,7 +2983,7 @@
       </c>
     </row>
     <row r="72" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="22" t="s">
+      <c r="A72" s="20" t="s">
         <v>56</v>
       </c>
       <c r="B72" s="14"/>
@@ -3007,7 +3016,7 @@
       </c>
     </row>
     <row r="73" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="22" t="s">
+      <c r="A73" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B73" s="14"/>
@@ -3039,14 +3048,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B74" s="14"/>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" s="21" t="s">
+        <v>109</v>
+      </c>
       <c r="C74" s="14">
         <f t="shared" si="12"/>
-        <v>2.3895457373988798</v>
+        <v>2.3762376237623761</v>
       </c>
       <c r="D74" s="14">
         <v>1</v>
@@ -3055,7 +3063,7 @@
         <v>3840</v>
       </c>
       <c r="F74" s="14">
-        <v>1607</v>
+        <v>1616</v>
       </c>
       <c r="G74" s="15" t="s">
         <v>9</v>
@@ -3065,21 +3073,21 @@
       </c>
       <c r="I74" s="14">
         <f t="shared" si="10"/>
-        <v>3840</v>
+        <v>240</v>
       </c>
       <c r="J74" s="14">
         <f t="shared" si="11"/>
-        <v>1607</v>
+        <v>101</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="22" t="s">
-        <v>59</v>
+      <c r="A75" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="B75" s="14"/>
       <c r="C75" s="14">
-        <f t="shared" si="12"/>
-        <v>2.4396442185514613</v>
+        <f>E75/F75</f>
+        <v>2.3895457373988798</v>
       </c>
       <c r="D75" s="14">
         <v>1</v>
@@ -3088,90 +3096,91 @@
         <v>3840</v>
       </c>
       <c r="F75" s="14">
+        <v>1607</v>
+      </c>
+      <c r="G75" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H75" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I75" s="14">
+        <f>LCM(E75*H75,F75*G75)/(F75*G75)</f>
+        <v>3840</v>
+      </c>
+      <c r="J75" s="14">
+        <f>LCM(E75*H75,F75*G75)/(E75*H75)</f>
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B76" s="14"/>
+      <c r="C76" s="14">
+        <f>E76/F76</f>
+        <v>2.4396442185514613</v>
+      </c>
+      <c r="D76" s="14">
+        <v>1</v>
+      </c>
+      <c r="E76" s="14">
+        <v>3840</v>
+      </c>
+      <c r="F76" s="14">
         <v>1574</v>
       </c>
-      <c r="G75" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H75" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I75" s="14">
-        <f t="shared" si="10"/>
+      <c r="G76" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H76" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I76" s="14">
+        <f>LCM(E76*H76,F76*G76)/(F76*G76)</f>
         <v>1920</v>
       </c>
-      <c r="J75" s="14">
-        <f t="shared" si="11"/>
+      <c r="J76" s="14">
+        <f>LCM(E76*H76,F76*G76)/(E76*H76)</f>
         <v>787</v>
       </c>
     </row>
-    <row r="76" spans="1:10" s="13" customFormat="1" ht="27" x14ac:dyDescent="0.3">
-      <c r="A76" s="16" t="s">
+    <row r="77" spans="1:10" s="13" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+      <c r="A77" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B76" s="17"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="17"/>
-      <c r="G76" s="18"/>
-      <c r="H76" s="18"/>
-      <c r="I76" s="17"/>
-      <c r="J76" s="17"/>
-    </row>
-    <row r="77" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="B77" s="14"/>
-      <c r="C77" s="14"/>
-      <c r="D77" s="14"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="15"/>
-      <c r="H77" s="15"/>
-      <c r="I77" s="14"/>
-      <c r="J77" s="14"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="18"/>
+      <c r="H77" s="18"/>
+      <c r="I77" s="17"/>
+      <c r="J77" s="17"/>
     </row>
     <row r="78" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="22" t="s">
+      <c r="A78" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B78" s="14"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="15"/>
+      <c r="H78" s="15"/>
+      <c r="I78" s="14"/>
+      <c r="J78" s="14"/>
+    </row>
+    <row r="79" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="20" t="s">
         <v>61</v>
-      </c>
-      <c r="B78" s="14"/>
-      <c r="C78" s="14">
-        <v>4</v>
-      </c>
-      <c r="D78" s="14">
-        <v>3</v>
-      </c>
-      <c r="E78" s="14">
-        <v>2048</v>
-      </c>
-      <c r="F78" s="14">
-        <v>1536</v>
-      </c>
-      <c r="G78" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H78" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I78" s="14">
-        <f t="shared" ref="I78:I86" si="13">LCM(E78*H78,F78*G78)/(F78*G78)</f>
-        <v>4</v>
-      </c>
-      <c r="J78" s="14">
-        <f t="shared" ref="J78:J86" si="14">LCM(E78*H78,F78*G78)/(E78*H78)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="22" t="s">
-        <v>62</v>
       </c>
       <c r="B79" s="14"/>
       <c r="C79" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D79" s="14">
         <v>3</v>
@@ -3180,129 +3189,128 @@
         <v>2048</v>
       </c>
       <c r="F79" s="14">
+        <v>1536</v>
+      </c>
+      <c r="G79" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H79" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I79" s="14">
+        <f t="shared" ref="I79:I87" si="13">LCM(E79*H79,F79*G79)/(F79*G79)</f>
+        <v>4</v>
+      </c>
+      <c r="J79" s="14">
+        <f t="shared" ref="J79:J87" si="14">LCM(E79*H79,F79*G79)/(E79*H79)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B80" s="14"/>
+      <c r="C80" s="14">
+        <v>5</v>
+      </c>
+      <c r="D80" s="14">
+        <v>3</v>
+      </c>
+      <c r="E80" s="14">
+        <v>2048</v>
+      </c>
+      <c r="F80" s="14">
         <v>1229</v>
       </c>
-      <c r="G79" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H79" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I79" s="14">
+      <c r="G80" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H80" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I80" s="14">
         <f t="shared" si="13"/>
         <v>2048</v>
       </c>
-      <c r="J79" s="14">
+      <c r="J80" s="14">
         <f t="shared" si="14"/>
         <v>1229</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A80" s="22" t="s">
+    <row r="81" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A81" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B80" s="14"/>
-      <c r="C80" s="14">
+      <c r="B81" s="14"/>
+      <c r="C81" s="14">
         <v>16</v>
       </c>
-      <c r="D80" s="14">
-        <v>9</v>
-      </c>
-      <c r="E80" s="14">
+      <c r="D81" s="14">
+        <v>9</v>
+      </c>
+      <c r="E81" s="14">
         <v>2048</v>
       </c>
-      <c r="F80" s="14">
+      <c r="F81" s="14">
         <v>1152</v>
       </c>
-      <c r="G80" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H80" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I80" s="14">
+      <c r="G81" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H81" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I81" s="14">
         <f t="shared" si="13"/>
         <v>16</v>
       </c>
-      <c r="J80" s="14">
+      <c r="J81" s="14">
         <f t="shared" si="14"/>
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="22" t="s">
+    <row r="82" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A82" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B81" s="14"/>
-      <c r="C81" s="14">
-        <f t="shared" ref="C78:C86" si="15">E81/F81</f>
+      <c r="B82" s="14"/>
+      <c r="C82" s="14">
+        <f t="shared" ref="C82:C87" si="15">E82/F82</f>
         <v>1.8500451671183378</v>
       </c>
-      <c r="D81" s="14">
-        <v>1</v>
-      </c>
-      <c r="E81" s="14">
+      <c r="D82" s="14">
+        <v>1</v>
+      </c>
+      <c r="E82" s="14">
         <v>2048</v>
       </c>
-      <c r="F81" s="14">
+      <c r="F82" s="14">
         <v>1107</v>
       </c>
-      <c r="G81" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H81" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I81" s="14">
+      <c r="G82" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H82" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I82" s="14">
         <f t="shared" si="13"/>
         <v>2048</v>
       </c>
-      <c r="J81" s="14">
+      <c r="J82" s="14">
         <f t="shared" si="14"/>
         <v>1107</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" s="22" t="s">
+    <row r="83" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A83" s="20" t="s">
         <v>65</v>
-      </c>
-      <c r="B82" s="14"/>
-      <c r="C82" s="14">
-        <f t="shared" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="D82" s="14">
-        <v>1</v>
-      </c>
-      <c r="E82" s="14">
-        <v>2048</v>
-      </c>
-      <c r="F82" s="14">
-        <v>1024</v>
-      </c>
-      <c r="G82" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H82" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I82" s="14">
-        <f t="shared" si="13"/>
-        <v>2</v>
-      </c>
-      <c r="J82" s="14">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" s="22" t="s">
-        <v>66</v>
       </c>
       <c r="B83" s="14"/>
       <c r="C83" s="14">
         <f t="shared" si="15"/>
-        <v>2.3513203214695753</v>
+        <v>2</v>
       </c>
       <c r="D83" s="14">
         <v>1</v>
@@ -3311,7 +3319,7 @@
         <v>2048</v>
       </c>
       <c r="F83" s="14">
-        <v>871</v>
+        <v>1024</v>
       </c>
       <c r="G83" s="15" t="s">
         <v>9</v>
@@ -3321,23 +3329,21 @@
       </c>
       <c r="I83" s="14">
         <f t="shared" si="13"/>
-        <v>2048</v>
+        <v>2</v>
       </c>
       <c r="J83" s="14">
         <f t="shared" si="14"/>
-        <v>871</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="B84" s="14" t="s">
-        <v>68</v>
-      </c>
+      <c r="A84" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B84" s="14"/>
       <c r="C84" s="14">
         <f t="shared" si="15"/>
-        <v>2.3703703703703702</v>
+        <v>2.3513203214695753</v>
       </c>
       <c r="D84" s="14">
         <v>1</v>
@@ -3346,7 +3352,7 @@
         <v>2048</v>
       </c>
       <c r="F84" s="14">
-        <v>864</v>
+        <v>871</v>
       </c>
       <c r="G84" s="15" t="s">
         <v>9</v>
@@ -3356,21 +3362,23 @@
       </c>
       <c r="I84" s="14">
         <f t="shared" si="13"/>
-        <v>64</v>
+        <v>2048</v>
       </c>
       <c r="J84" s="14">
         <f t="shared" si="14"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A85" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="B85" s="14"/>
+        <v>871</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B85" s="14" t="s">
+        <v>68</v>
+      </c>
       <c r="C85" s="14">
         <f t="shared" si="15"/>
-        <v>2.3869463869463869</v>
+        <v>2.3703703703703702</v>
       </c>
       <c r="D85" s="14">
         <v>1</v>
@@ -3379,7 +3387,7 @@
         <v>2048</v>
       </c>
       <c r="F85" s="14">
-        <v>858</v>
+        <v>864</v>
       </c>
       <c r="G85" s="15" t="s">
         <v>9</v>
@@ -3389,21 +3397,21 @@
       </c>
       <c r="I85" s="14">
         <f t="shared" si="13"/>
-        <v>1024</v>
+        <v>64</v>
       </c>
       <c r="J85" s="14">
         <f t="shared" si="14"/>
-        <v>429</v>
+        <v>27</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" s="22" t="s">
-        <v>70</v>
+      <c r="A86" s="20" t="s">
+        <v>69</v>
       </c>
       <c r="B86" s="14"/>
       <c r="C86" s="14">
         <f t="shared" si="15"/>
-        <v>2.4410011918951131</v>
+        <v>2.3869463869463869</v>
       </c>
       <c r="D86" s="14">
         <v>1</v>
@@ -3412,7 +3420,7 @@
         <v>2048</v>
       </c>
       <c r="F86" s="14">
-        <v>839</v>
+        <v>858</v>
       </c>
       <c r="G86" s="15" t="s">
         <v>9</v>
@@ -3422,417 +3430,417 @@
       </c>
       <c r="I86" s="14">
         <f t="shared" si="13"/>
-        <v>2048</v>
+        <v>1024</v>
       </c>
       <c r="J86" s="14">
         <f t="shared" si="14"/>
+        <v>429</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A87" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B87" s="14"/>
+      <c r="C87" s="14">
+        <f t="shared" si="15"/>
+        <v>2.4410011918951131</v>
+      </c>
+      <c r="D87" s="14">
+        <v>1</v>
+      </c>
+      <c r="E87" s="14">
+        <v>2048</v>
+      </c>
+      <c r="F87" s="14">
         <v>839</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" s="13" customFormat="1" ht="27" x14ac:dyDescent="0.3">
-      <c r="A87" s="16" t="s">
+      <c r="G87" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H87" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I87" s="14">
+        <f t="shared" si="13"/>
+        <v>2048</v>
+      </c>
+      <c r="J87" s="14">
+        <f t="shared" si="14"/>
+        <v>839</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" s="13" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+      <c r="A88" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B87" s="17"/>
-      <c r="C87" s="17"/>
-      <c r="D87" s="17"/>
-      <c r="E87" s="17"/>
-      <c r="F87" s="17"/>
-      <c r="G87" s="18"/>
-      <c r="H87" s="18"/>
-      <c r="I87" s="17"/>
-      <c r="J87" s="17"/>
-    </row>
-    <row r="88" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="B88" s="14"/>
-      <c r="C88" s="14"/>
-      <c r="D88" s="14"/>
-      <c r="E88" s="14"/>
-      <c r="F88" s="14"/>
-      <c r="G88" s="15"/>
-      <c r="H88" s="15"/>
-      <c r="I88" s="14"/>
-      <c r="J88" s="14"/>
+      <c r="B88" s="17"/>
+      <c r="C88" s="17"/>
+      <c r="D88" s="17"/>
+      <c r="E88" s="17"/>
+      <c r="F88" s="17"/>
+      <c r="G88" s="18"/>
+      <c r="H88" s="18"/>
+      <c r="I88" s="17"/>
+      <c r="J88" s="17"/>
     </row>
     <row r="89" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" s="22" t="s">
+      <c r="A89" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B89" s="14"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="15"/>
+      <c r="H89" s="15"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="14"/>
+    </row>
+    <row r="90" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A90" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="B89" s="14"/>
-      <c r="C89" s="23">
-        <f t="shared" ref="C89:C94" si="16">LCM(E89,F89)/F89</f>
+      <c r="B90" s="14"/>
+      <c r="C90" s="21">
+        <f t="shared" ref="C90:C95" si="16">LCM(E90,F90)/F90</f>
         <v>64</v>
       </c>
-      <c r="D89" s="14">
-        <f t="shared" ref="D89:D94" si="17">LCM(E89,F89)/E89</f>
+      <c r="D90" s="14">
+        <f t="shared" ref="D90:D95" si="17">LCM(E90,F90)/E90</f>
         <v>27</v>
       </c>
-      <c r="E89" s="14">
+      <c r="E90" s="14">
         <v>2560</v>
       </c>
-      <c r="F89" s="14">
+      <c r="F90" s="14">
         <v>1080</v>
       </c>
-      <c r="G89" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H89" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I89" s="14">
-        <f>LCM(E89,F89,G89,H89)/(F89*G89)</f>
+      <c r="G90" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H90" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I90" s="14">
+        <f>LCM(E90,F90,G90,H90)/(F90*G90)</f>
         <v>64</v>
       </c>
-      <c r="J89" s="14">
-        <f>LCM(E89,F89,G89,H89)/(E89*H89)</f>
+      <c r="J90" s="14">
+        <f>LCM(E90,F90,G90,H90)/(E90*H90)</f>
         <v>27</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A90" s="19"/>
-      <c r="B90" s="14"/>
-      <c r="C90" s="23">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A91" s="19"/>
+      <c r="B91" s="14"/>
+      <c r="C91" s="21">
         <f t="shared" si="16"/>
         <v>64</v>
       </c>
-      <c r="D90" s="14">
+      <c r="D91" s="14">
         <f t="shared" si="17"/>
         <v>27</v>
       </c>
-      <c r="E90" s="14">
+      <c r="E91" s="14">
         <v>2560</v>
       </c>
-      <c r="F90" s="14">
+      <c r="F91" s="14">
         <v>1080</v>
       </c>
-      <c r="G90" s="15" t="s">
+      <c r="G91" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H90" s="15" t="s">
+      <c r="H91" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="I90" s="14">
-        <f>LCM(E90,F90,G90,H90)/(F90*G90)</f>
+      <c r="I91" s="14">
+        <f>LCM(E91,F91,G91,H91)/(F91*G91)</f>
         <v>16</v>
       </c>
-      <c r="J90" s="14">
-        <f>LCM(E90,F90,G90,H90)/(E90*H90)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A91" s="22" t="s">
+      <c r="J91" s="14">
+        <f>LCM(E91,F91,G91,H91)/(E91*H91)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A92" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="B91" s="14"/>
-      <c r="C91" s="23">
+      <c r="B92" s="14"/>
+      <c r="C92" s="21">
         <f t="shared" si="16"/>
         <v>5</v>
       </c>
-      <c r="D91" s="14">
+      <c r="D92" s="14">
         <f t="shared" si="17"/>
         <v>3</v>
       </c>
-      <c r="E91" s="14">
+      <c r="E92" s="14">
         <v>1920</v>
       </c>
-      <c r="F91" s="14">
+      <c r="F92" s="14">
         <v>1152</v>
       </c>
-      <c r="G91" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H91" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I91" s="14">
-        <f>LCM(E91,F91,G91,H91)/(F91*G91)</f>
+      <c r="G92" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H92" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I92" s="14">
+        <f>LCM(E92,F92,G92,H92)/(F92*G92)</f>
         <v>5</v>
       </c>
-      <c r="J91" s="14">
-        <f>LCM(E91,F91,G91,H91)/(E91*H91)</f>
+      <c r="J92" s="14">
+        <f>LCM(E92,F92,G92,H92)/(E92*H92)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A92" s="22" t="s">
+    <row r="93" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A93" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="B92" s="14" t="s">
+      <c r="B93" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C92" s="23">
+      <c r="C93" s="21">
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-      <c r="D92" s="14">
+      <c r="D93" s="14">
         <f t="shared" si="17"/>
         <v>9</v>
       </c>
-      <c r="E92" s="14">
+      <c r="E93" s="14">
         <v>1920</v>
       </c>
-      <c r="F92" s="14">
+      <c r="F93" s="14">
         <v>1080</v>
       </c>
-      <c r="G92" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H92" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I92" s="14">
-        <f t="shared" ref="I92:I109" si="18">LCM(E92*H92,F92*G92)/(F92*G92)</f>
+      <c r="G93" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H93" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I93" s="14">
+        <f t="shared" ref="I93:I110" si="18">LCM(E93*H93,F93*G93)/(F93*G93)</f>
         <v>16</v>
       </c>
-      <c r="J92" s="14">
-        <f t="shared" ref="J92:J109" si="19">LCM(E92*H92,F92*G92)/(E92*H92)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A93" s="22"/>
-      <c r="B93" s="14" t="s">
+      <c r="J93" s="14">
+        <f t="shared" ref="J93:J110" si="19">LCM(E93*H93,F93*G93)/(E93*H93)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A94" s="20"/>
+      <c r="B94" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C93" s="23">
+      <c r="C94" s="21">
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-      <c r="D93" s="14">
+      <c r="D94" s="14">
         <f t="shared" si="17"/>
         <v>9</v>
       </c>
-      <c r="E93" s="14">
+      <c r="E94" s="14">
         <v>1920</v>
       </c>
-      <c r="F93" s="14">
+      <c r="F94" s="14">
         <v>1080</v>
       </c>
-      <c r="G93" s="15" t="s">
+      <c r="G94" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H93" s="15" t="s">
+      <c r="H94" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I93" s="14">
+      <c r="I94" s="14">
         <f t="shared" si="18"/>
         <v>1</v>
       </c>
-      <c r="J93" s="14">
+      <c r="J94" s="14">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A94" s="22"/>
-      <c r="B94" s="14" t="s">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A95" s="20"/>
+      <c r="B95" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C94" s="23">
+      <c r="C95" s="21">
         <f t="shared" si="16"/>
         <v>16</v>
       </c>
-      <c r="D94" s="14">
+      <c r="D95" s="14">
         <f t="shared" si="17"/>
         <v>9</v>
       </c>
-      <c r="E94" s="14">
+      <c r="E95" s="14">
         <v>1920</v>
       </c>
-      <c r="F94" s="14">
+      <c r="F95" s="14">
         <v>1080</v>
       </c>
-      <c r="G94" s="15" t="s">
+      <c r="G95" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H94" s="15" t="s">
+      <c r="H95" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="I94" s="14">
+      <c r="I95" s="14">
         <f t="shared" si="18"/>
         <v>4</v>
       </c>
-      <c r="J94" s="14">
+      <c r="J95" s="14">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A95" s="22" t="s">
+    <row r="96" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B95" s="14" t="s">
+      <c r="B96" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C95" s="14">
-        <f>E95/F95</f>
+      <c r="C96" s="14">
+        <f>E96/F96</f>
         <v>1.8497109826589595</v>
       </c>
-      <c r="D95" s="14">
-        <v>1</v>
-      </c>
-      <c r="E95" s="14">
+      <c r="D96" s="14">
+        <v>1</v>
+      </c>
+      <c r="E96" s="14">
         <v>1920</v>
       </c>
-      <c r="F95" s="14">
+      <c r="F96" s="14">
         <v>1038</v>
       </c>
-      <c r="G95" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H95" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I95" s="14">
+      <c r="G96" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H96" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I96" s="14">
         <f t="shared" si="18"/>
         <v>320</v>
       </c>
-      <c r="J95" s="14">
+      <c r="J96" s="14">
         <f t="shared" si="19"/>
         <v>173</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A96" s="22" t="s">
+    <row r="97" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B96" s="14"/>
-      <c r="C96" s="23">
-        <f>LCM(E96,F96)/F96</f>
+      <c r="B97" s="14"/>
+      <c r="C97" s="21">
+        <f>LCM(E97,F97)/F97</f>
         <v>2</v>
       </c>
-      <c r="D96" s="14">
-        <f>LCM(E96,F96)/E96</f>
-        <v>1</v>
-      </c>
-      <c r="E96" s="14">
+      <c r="D97" s="14">
+        <f>LCM(E97,F97)/E97</f>
+        <v>1</v>
+      </c>
+      <c r="E97" s="14">
         <v>1920</v>
       </c>
-      <c r="F96" s="14">
+      <c r="F97" s="14">
         <v>960</v>
       </c>
-      <c r="G96" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H96" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I96" s="14">
+      <c r="G97" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H97" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I97" s="14">
         <f t="shared" si="18"/>
         <v>2</v>
       </c>
-      <c r="J96" s="14">
+      <c r="J97" s="14">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A97" s="22" t="s">
+    <row r="98" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B97" s="14"/>
-      <c r="C97" s="14">
-        <f t="shared" ref="C97:C103" si="20">E97/F97</f>
+      <c r="B98" s="14"/>
+      <c r="C98" s="14">
+        <f t="shared" ref="C98:C104" si="20">E98/F98</f>
         <v>2.3500611995104039</v>
       </c>
-      <c r="D97" s="14">
-        <v>1</v>
-      </c>
-      <c r="E97" s="14">
+      <c r="D98" s="14">
+        <v>1</v>
+      </c>
+      <c r="E98" s="14">
         <v>1920</v>
       </c>
-      <c r="F97" s="14">
+      <c r="F98" s="14">
         <v>817</v>
       </c>
-      <c r="G97" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H97" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I97" s="14">
+      <c r="G98" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H98" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I98" s="14">
         <f t="shared" si="18"/>
         <v>1920</v>
       </c>
-      <c r="J97" s="14">
+      <c r="J98" s="14">
         <f t="shared" si="19"/>
         <v>817</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A98" s="22" t="s">
+    <row r="99" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B98" s="14"/>
-      <c r="C98" s="14">
+      <c r="B99" s="14"/>
+      <c r="C99" s="14">
         <f t="shared" si="20"/>
         <v>2.3529411764705883</v>
       </c>
-      <c r="D98" s="14">
-        <v>1</v>
-      </c>
-      <c r="E98" s="14">
+      <c r="D99" s="14">
+        <v>1</v>
+      </c>
+      <c r="E99" s="14">
         <v>1920</v>
       </c>
-      <c r="F98" s="14">
+      <c r="F99" s="14">
         <v>816</v>
       </c>
-      <c r="G98" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H98" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I98" s="14">
+      <c r="G99" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H99" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I99" s="14">
         <f t="shared" si="18"/>
         <v>40</v>
       </c>
-      <c r="J98" s="14">
+      <c r="J99" s="14">
         <f t="shared" si="19"/>
         <v>17</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A99" s="22" t="s">
+    <row r="100" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B99" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C99" s="14">
-        <f t="shared" si="20"/>
-        <v>2.3703703703703702</v>
-      </c>
-      <c r="D99" s="14">
-        <v>1</v>
-      </c>
-      <c r="E99" s="14">
-        <v>1920</v>
-      </c>
-      <c r="F99" s="14">
-        <v>810</v>
-      </c>
-      <c r="G99" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H99" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I99" s="14">
-        <f t="shared" si="18"/>
-        <v>64</v>
-      </c>
-      <c r="J99" s="14">
-        <f t="shared" si="19"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A100" s="22"/>
       <c r="B100" s="14" t="s">
         <v>68</v>
       </c>
@@ -3850,22 +3858,22 @@
         <v>810</v>
       </c>
       <c r="G100" s="15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H100" s="15" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I100" s="14">
         <f t="shared" si="18"/>
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="J100" s="14">
         <f t="shared" si="19"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A101" s="22"/>
+      <c r="A101" s="20"/>
       <c r="B101" s="14" t="s">
         <v>68</v>
       </c>
@@ -3883,28 +3891,28 @@
         <v>810</v>
       </c>
       <c r="G101" s="15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H101" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I101" s="14">
         <f t="shared" si="18"/>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="J101" s="14">
         <f t="shared" si="19"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A102" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="B102" s="14"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A102" s="20"/>
+      <c r="B102" s="14" t="s">
+        <v>68</v>
+      </c>
       <c r="C102" s="14">
         <f t="shared" si="20"/>
-        <v>2.391033623910336</v>
+        <v>2.3703703703703702</v>
       </c>
       <c r="D102" s="14">
         <v>1</v>
@@ -3913,33 +3921,31 @@
         <v>1920</v>
       </c>
       <c r="F102" s="14">
-        <v>803</v>
+        <v>810</v>
       </c>
       <c r="G102" s="15" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="H102" s="15" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I102" s="14">
         <f t="shared" si="18"/>
-        <v>1920</v>
+        <v>16</v>
       </c>
       <c r="J102" s="14">
         <f t="shared" si="19"/>
-        <v>803</v>
+        <v>9</v>
       </c>
     </row>
     <row r="103" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A103" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="B103" s="14" t="s">
-        <v>83</v>
-      </c>
+      <c r="A103" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B103" s="14"/>
       <c r="C103" s="14">
         <f t="shared" si="20"/>
-        <v>2.4</v>
+        <v>2.391033623910336</v>
       </c>
       <c r="D103" s="14">
         <v>1</v>
@@ -3948,7 +3954,7 @@
         <v>1920</v>
       </c>
       <c r="F103" s="14">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="G103" s="15" t="s">
         <v>9</v>
@@ -3958,56 +3964,55 @@
       </c>
       <c r="I103" s="14">
         <f t="shared" si="18"/>
-        <v>12</v>
+        <v>1920</v>
       </c>
       <c r="J103" s="14">
         <f t="shared" si="19"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A104" s="22"/>
+        <v>803</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A104" s="20" t="s">
+        <v>106</v>
+      </c>
       <c r="B104" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C104" s="14">
-        <f t="shared" ref="C104:F105" si="21">C103</f>
+        <f t="shared" si="20"/>
         <v>2.4</v>
       </c>
       <c r="D104" s="14">
-        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="E104" s="14">
-        <f t="shared" si="21"/>
         <v>1920</v>
       </c>
       <c r="F104" s="14">
-        <f t="shared" si="21"/>
         <v>800</v>
       </c>
       <c r="G104" s="15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H104" s="15" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I104" s="14">
         <f t="shared" si="18"/>
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="J104" s="14">
         <f t="shared" si="19"/>
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A105" s="22"/>
+      <c r="A105" s="20"/>
       <c r="B105" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C105" s="14">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="C105:F106" si="21">C104</f>
         <v>2.4</v>
       </c>
       <c r="D105" s="14">
@@ -4023,71 +4028,73 @@
         <v>800</v>
       </c>
       <c r="G105" s="15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H105" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I105" s="14">
         <f t="shared" si="18"/>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="J105" s="14">
         <f t="shared" si="19"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A106" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="B106" s="14"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A106" s="20"/>
+      <c r="B106" s="14" t="s">
+        <v>82</v>
+      </c>
       <c r="C106" s="14">
-        <f>E106/F106</f>
-        <v>2.4396442185514613</v>
+        <f t="shared" si="21"/>
+        <v>2.4</v>
       </c>
       <c r="D106" s="14">
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="E106" s="14">
+        <f t="shared" si="21"/>
         <v>1920</v>
       </c>
       <c r="F106" s="14">
-        <v>787</v>
+        <f t="shared" si="21"/>
+        <v>800</v>
       </c>
       <c r="G106" s="15" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="H106" s="15" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I106" s="14">
         <f t="shared" si="18"/>
-        <v>1920</v>
+        <v>9</v>
       </c>
       <c r="J106" s="14">
         <f t="shared" si="19"/>
-        <v>787</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" s="22" t="s">
-        <v>85</v>
+      <c r="A107" s="20" t="s">
+        <v>83</v>
       </c>
       <c r="B107" s="14"/>
-      <c r="C107" s="23">
-        <f>LCM(E107,F107)/F107</f>
-        <v>4</v>
+      <c r="C107" s="14">
+        <f>E107/F107</f>
+        <v>2.4396442185514613</v>
       </c>
       <c r="D107" s="14">
-        <f>LCM(E107,F107)/E107</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E107" s="14">
         <v>1920</v>
       </c>
       <c r="F107" s="14">
-        <v>1440</v>
+        <v>787</v>
       </c>
       <c r="G107" s="15" t="s">
         <v>9</v>
@@ -4097,17 +4104,19 @@
       </c>
       <c r="I107" s="14">
         <f t="shared" si="18"/>
-        <v>4</v>
+        <v>1920</v>
       </c>
       <c r="J107" s="14">
         <f t="shared" si="19"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A108" s="22"/>
+        <v>787</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="B108" s="14"/>
-      <c r="C108" s="23">
+      <c r="C108" s="21">
         <f>LCM(E108,F108)/F108</f>
         <v>4</v>
       </c>
@@ -4122,24 +4131,24 @@
         <v>1440</v>
       </c>
       <c r="G108" s="15" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H108" s="15" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I108" s="14">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J108" s="14">
         <f t="shared" si="19"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A109" s="22"/>
+      <c r="A109" s="20"/>
       <c r="B109" s="14"/>
-      <c r="C109" s="23">
+      <c r="C109" s="21">
         <f>LCM(E109,F109)/F109</f>
         <v>4</v>
       </c>
@@ -4154,92 +4163,104 @@
         <v>1440</v>
       </c>
       <c r="G109" s="15" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H109" s="15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I109" s="14">
         <f t="shared" si="18"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J109" s="14">
         <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A110" s="20"/>
+      <c r="B110" s="14"/>
+      <c r="C110" s="21">
+        <f>LCM(E110,F110)/F110</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A110" s="12"/>
-      <c r="C110" s="5"/>
-    </row>
-    <row r="111" spans="1:10" s="13" customFormat="1" ht="27" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
-      <c r="D111" s="2"/>
-      <c r="E111" s="2"/>
-      <c r="F111" s="2"/>
-      <c r="G111" s="3"/>
-      <c r="H111" s="3"/>
-      <c r="I111" s="2"/>
-      <c r="J111" s="2"/>
-    </row>
-    <row r="112" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A112" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="B112" s="4"/>
-      <c r="C112" s="4"/>
-      <c r="D112" s="4"/>
-      <c r="E112" s="4"/>
-      <c r="F112" s="4"/>
-      <c r="G112" s="7"/>
-      <c r="H112" s="7"/>
-      <c r="I112" s="4"/>
-      <c r="J112" s="4"/>
-    </row>
-    <row r="113" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A113" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B113" s="4"/>
-      <c r="C113" s="11">
-        <f>LCM(E113,F113)/F113</f>
+      <c r="D110" s="14">
+        <f>LCM(E110,F110)/E110</f>
+        <v>3</v>
+      </c>
+      <c r="E110" s="14">
+        <v>1920</v>
+      </c>
+      <c r="F110" s="14">
+        <v>1440</v>
+      </c>
+      <c r="G110" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H110" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I110" s="14">
+        <f t="shared" si="18"/>
+        <v>3</v>
+      </c>
+      <c r="J110" s="14">
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="D113" s="4">
-        <f>LCM(E113,F113)/E113</f>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A111" s="12"/>
+      <c r="C111" s="5"/>
+    </row>
+    <row r="112" spans="1:10" s="13" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B112" s="2"/>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
+      <c r="G112" s="3"/>
+      <c r="H112" s="3"/>
+      <c r="I112" s="2"/>
+      <c r="J112" s="2"/>
+    </row>
+    <row r="113" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B113" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C113" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D113" s="28"/>
+      <c r="E113" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E113" s="4">
-        <v>1280</v>
-      </c>
-      <c r="F113" s="4">
-        <v>960</v>
-      </c>
-      <c r="G113" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H113" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I113" s="4">
-        <v>1</v>
-      </c>
-      <c r="J113" s="4">
-        <v>1</v>
-      </c>
+      <c r="F113" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G113" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="H113" s="29"/>
+      <c r="I113" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="J113" s="28"/>
     </row>
     <row r="114" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B114" s="4"/>
       <c r="C114" s="11">
         <f>LCM(E114,F114)/F114</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D114" s="4">
         <f>LCM(E114,F114)/E114</f>
@@ -4249,7 +4270,7 @@
         <v>1280</v>
       </c>
       <c r="F114" s="4">
-        <v>768</v>
+        <v>960</v>
       </c>
       <c r="G114" s="7" t="s">
         <v>9</v>
@@ -4266,24 +4287,22 @@
     </row>
     <row r="115" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>90</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B115" s="4"/>
       <c r="C115" s="11">
         <f>LCM(E115,F115)/F115</f>
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D115" s="4">
         <f>LCM(E115,F115)/E115</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E115" s="4">
         <v>1280</v>
       </c>
       <c r="F115" s="4">
-        <v>720</v>
+        <v>768</v>
       </c>
       <c r="G115" s="7" t="s">
         <v>9</v>
@@ -4298,10 +4317,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A116" s="6"/>
+    <row r="116" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A116" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="B116" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C116" s="11">
         <f>LCM(E116,F116)/F116</f>
@@ -4318,10 +4339,10 @@
         <v>720</v>
       </c>
       <c r="G116" s="7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H116" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I116" s="4">
         <v>1</v>
@@ -4330,149 +4351,141 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A117" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B117" s="4"/>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A117" s="6"/>
+      <c r="B117" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="C117" s="11">
         <f>LCM(E117,F117)/F117</f>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D117" s="4">
         <f>LCM(E117,F117)/E117</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E117" s="4">
-        <v>1680</v>
+        <v>1280</v>
       </c>
       <c r="F117" s="4">
         <v>720</v>
       </c>
       <c r="G117" s="7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="H117" s="7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I117" s="4">
-        <f t="shared" ref="I117:I123" si="22">LCM(E117*H117,F117*G117)/(F117*G117)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J117" s="4">
-        <f t="shared" ref="J117:J123" si="23">LCM(E117*H117,F117*G117)/(E117*H117)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="6" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="B118" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C118" s="11">
+        <f>LCM(E118,F118)/F118</f>
+        <v>7</v>
+      </c>
+      <c r="D118" s="4">
+        <f>LCM(E118,F118)/E118</f>
+        <v>3</v>
+      </c>
+      <c r="E118" s="4">
+        <v>1680</v>
+      </c>
+      <c r="F118" s="4">
+        <v>720</v>
+      </c>
+      <c r="G118" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H118" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I118" s="4">
+        <f t="shared" ref="I118:I125" si="22">LCM(E118*H118,F118*G118)/(F118*G118)</f>
+        <v>7</v>
+      </c>
+      <c r="J118" s="4">
+        <f t="shared" ref="J118:J125" si="23">LCM(E118*H118,F118*G118)/(E118*H118)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A119" s="6"/>
+      <c r="B119" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C119" s="11"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="4"/>
+      <c r="G119" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H119" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I119" s="14" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J119" s="14" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A120" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B120" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C118" s="4">
-        <f t="shared" ref="C118:C123" si="24">E118/F118</f>
+      <c r="C120" s="4">
+        <f t="shared" ref="C120:C125" si="24">E120/F120</f>
         <v>1.8497109826589595</v>
       </c>
-      <c r="D118" s="4">
-        <v>1</v>
-      </c>
-      <c r="E118" s="4">
+      <c r="D120" s="4">
+        <v>1</v>
+      </c>
+      <c r="E120" s="4">
         <v>1280</v>
       </c>
-      <c r="F118" s="4">
+      <c r="F120" s="4">
         <v>692</v>
       </c>
-      <c r="G118" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H118" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I118" s="4">
+      <c r="G120" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H120" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I120" s="4">
         <f t="shared" si="22"/>
         <v>320</v>
       </c>
-      <c r="J118" s="4">
+      <c r="J120" s="4">
         <f t="shared" si="23"/>
         <v>173</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A119" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B119" s="4"/>
-      <c r="C119" s="4">
-        <f t="shared" si="24"/>
-        <v>2</v>
-      </c>
-      <c r="D119" s="4">
-        <v>1</v>
-      </c>
-      <c r="E119" s="4">
-        <v>1280</v>
-      </c>
-      <c r="F119" s="4">
-        <v>640</v>
-      </c>
-      <c r="G119" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H119" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I119" s="4">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="J119" s="4">
-        <f t="shared" si="23"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A120" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B120" s="4"/>
-      <c r="C120" s="4">
-        <f t="shared" si="24"/>
-        <v>2.3486238532110093</v>
-      </c>
-      <c r="D120" s="4">
-        <v>1</v>
-      </c>
-      <c r="E120" s="4">
-        <v>1280</v>
-      </c>
-      <c r="F120" s="4">
-        <v>545</v>
-      </c>
-      <c r="G120" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H120" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I120" s="4">
-        <f t="shared" si="22"/>
-        <v>256</v>
-      </c>
-      <c r="J120" s="4">
-        <f t="shared" si="23"/>
-        <v>109</v>
-      </c>
-    </row>
     <row r="121" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B121" s="4"/>
       <c r="C121" s="4">
         <f t="shared" si="24"/>
-        <v>2.3703703703703702</v>
+        <v>2</v>
       </c>
       <c r="D121" s="4">
         <v>1</v>
@@ -4481,7 +4494,7 @@
         <v>1280</v>
       </c>
       <c r="F121" s="4">
-        <v>540</v>
+        <v>640</v>
       </c>
       <c r="G121" s="7" t="s">
         <v>9</v>
@@ -4491,21 +4504,21 @@
       </c>
       <c r="I121" s="4">
         <f t="shared" si="22"/>
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="J121" s="4">
         <f t="shared" si="23"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B122" s="4"/>
       <c r="C122" s="4">
         <f t="shared" si="24"/>
-        <v>2.3880597014925371</v>
+        <v>2.3486238532110093</v>
       </c>
       <c r="D122" s="4">
         <v>1</v>
@@ -4514,7 +4527,7 @@
         <v>1280</v>
       </c>
       <c r="F122" s="4">
-        <v>536</v>
+        <v>545</v>
       </c>
       <c r="G122" s="7" t="s">
         <v>9</v>
@@ -4524,21 +4537,21 @@
       </c>
       <c r="I122" s="4">
         <f t="shared" si="22"/>
-        <v>160</v>
+        <v>256</v>
       </c>
       <c r="J122" s="4">
         <f t="shared" si="23"/>
-        <v>67</v>
+        <v>109</v>
       </c>
     </row>
     <row r="123" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B123" s="4"/>
       <c r="C123" s="4">
         <f t="shared" si="24"/>
-        <v>2.4380952380952383</v>
+        <v>2.3703703703703702</v>
       </c>
       <c r="D123" s="4">
         <v>1</v>
@@ -4547,7 +4560,7 @@
         <v>1280</v>
       </c>
       <c r="F123" s="4">
-        <v>525</v>
+        <v>540</v>
       </c>
       <c r="G123" s="7" t="s">
         <v>9</v>
@@ -4557,33 +4570,102 @@
       </c>
       <c r="I123" s="4">
         <f t="shared" si="22"/>
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="J123" s="4">
         <f t="shared" si="23"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A124" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B124" s="4"/>
+      <c r="C124" s="4">
+        <f t="shared" si="24"/>
+        <v>2.3880597014925371</v>
+      </c>
+      <c r="D124" s="4">
+        <v>1</v>
+      </c>
+      <c r="E124" s="4">
+        <v>1280</v>
+      </c>
+      <c r="F124" s="4">
+        <v>536</v>
+      </c>
+      <c r="G124" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H124" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I124" s="4">
+        <f t="shared" si="22"/>
+        <v>160</v>
+      </c>
+      <c r="J124" s="4">
+        <f t="shared" si="23"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A125" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B125" s="4"/>
+      <c r="C125" s="4">
+        <f t="shared" si="24"/>
+        <v>2.4380952380952383</v>
+      </c>
+      <c r="D125" s="4">
+        <v>1</v>
+      </c>
+      <c r="E125" s="4">
+        <v>1280</v>
+      </c>
+      <c r="F125" s="4">
+        <v>525</v>
+      </c>
+      <c r="G125" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H125" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I125" s="4">
+        <f t="shared" si="22"/>
+        <v>256</v>
+      </c>
+      <c r="J125" s="4">
+        <f t="shared" si="23"/>
         <v>105</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A124" s="11"/>
-      <c r="B124" s="4"/>
-      <c r="C124" s="4"/>
-      <c r="D124" s="4"/>
-      <c r="E124" s="4"/>
-      <c r="F124" s="4"/>
-      <c r="G124" s="7"/>
-      <c r="H124" s="7"/>
-      <c r="I124" s="4"/>
-      <c r="J124" s="4"/>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A126" s="11"/>
+      <c r="B126" s="4"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="4"/>
+      <c r="F126" s="4"/>
+      <c r="G126" s="7"/>
+      <c r="H126" s="7"/>
+      <c r="I126" s="4"/>
+      <c r="J126" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="G113:H113"/>
+    <mergeCell ref="I113:J113"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="I10:J10"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>